<commit_message>
modified:   app/globals.css 	modified:   app/layout.tsx 	new file:   public/GST_Template (3).xlsx 	modified:   public/GST_Template.xlsx 	new file:   public/app_icon.png 	new file:   public/favicon.png 	modified:   scripts/update-template.js
</commit_message>
<xml_diff>
--- a/public/GST_Template.xlsx
+++ b/public/GST_Template.xlsx
@@ -76,9 +76,13 @@
   <cellStyleXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles>
@@ -100,45 +104,45 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Jpan" typeface="æ¸¸ã´ã·ãã¯ Light"/>
+        <a:font script="Hang" typeface="ë§ì ê³ ë"/>
+        <a:font script="Hans" typeface="ç­çº¿ Light"/>
+        <a:font script="Hant" typeface="æ°ç´°æé«"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -167,13 +171,13 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Jpan" typeface="æ¸¸ã´ã·ãã¯"/>
+        <a:font script="Hang" typeface="ë§ì ê³ ë"/>
+        <a:font script="Hans" typeface="ç­çº¿"/>
+        <a:font script="Hant" typeface="æ°ç´°æé«"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -211,201 +215,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -413,83 +358,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" customWidth="1" width="30"/>
+    <col min="2" max="2" customWidth="1" width="12"/>
+    <col min="3" max="3" customWidth="1" width="50"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="str">
+      <c r="A1" s="3" t="str">
         <v>Field</v>
       </c>
-      <c r="B1" s="2" t="str">
+      <c r="B1" s="3" t="str">
         <v>Mandatory</v>
       </c>
-      <c r="C1" s="2" t="str">
+      <c r="C1" s="3" t="str">
         <v>Format/Notes</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="str">
+      <c r="A2" s="4" t="str">
         <v>Invoice Date *</v>
       </c>
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="4" t="str">
         <v>Yes</v>
       </c>
-      <c r="C2" s="2" t="str">
+      <c r="C2" s="4" t="str">
         <v>DD-MM-YYYY</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="str">
+      <c r="A3" s="4" t="str">
         <v>Invoice No. *</v>
       </c>
-      <c r="B3" s="2" t="str">
+      <c r="B3" s="4" t="str">
         <v>Yes</v>
       </c>
-      <c r="C3" s="2" t="str">
+      <c r="C3" s="4" t="str">
         <v>Alphanumeric, Max 16 chars</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="str">
+      <c r="A4" s="4" t="str">
         <v>Billing GSTIN</v>
       </c>
-      <c r="B4" s="2" t="str">
+      <c r="B4" s="4" t="str">
         <v>B2B</v>
       </c>
-      <c r="C4" s="2" t="str">
+      <c r="C4" s="4" t="str">
         <v>15-character GSTIN</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="str">
+      <c r="A5" s="4" t="str">
         <v>Taxable Value *</v>
       </c>
-      <c r="B5" s="2" t="str">
+      <c r="B5" s="4" t="str">
         <v>Yes</v>
       </c>
-      <c r="C5" s="2" t="str">
+      <c r="C5" s="4" t="str">
         <v>Enter base amount (₹)</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="str">
+      <c r="A6" s="4" t="str">
         <v>CGST/SGST/IGST Rate</v>
       </c>
-      <c r="B6" s="2" t="str">
+      <c r="B6" s="4" t="str">
         <v>Select</v>
       </c>
-      <c r="C6" s="2" t="str">
+      <c r="C6" s="4" t="str">
         <v>Choose rate from dropdown - Amounts auto-calculate!</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="str">
+      <c r="A7" s="4" t="str">
         <v>Total Transaction Value</v>
       </c>
-      <c r="B7" s="2" t="str">
+      <c r="B7" s="4" t="str">
         <v>Auto</v>
       </c>
-      <c r="C7" s="2" t="str">
+      <c r="C7" s="4" t="str">
         <v>Auto-calculated: Taxable + CGST + SGST + IGST</v>
       </c>
     </row>
@@ -505,68 +455,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U500"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" customWidth="1" width="14"/>
+    <col min="2" max="2" customWidth="1" width="16"/>
+    <col min="3" max="3" customWidth="1" width="22"/>
+    <col min="4" max="4" customWidth="1" width="17"/>
+    <col min="5" max="5" customWidth="1" width="18"/>
+    <col min="6" max="6" customWidth="1" width="5"/>
+    <col min="7" max="7" customWidth="1" width="20"/>
+    <col min="8" max="8" customWidth="1" width="12"/>
+    <col min="9" max="9" customWidth="1" width="8"/>
+    <col min="10" max="10" customWidth="1" width="8"/>
+    <col min="11" max="11" customWidth="1" width="14"/>
+    <col min="12" max="12" customWidth="1" width="8"/>
+    <col min="13" max="13" customWidth="1" width="10"/>
+    <col min="14" max="14" customWidth="1" width="8"/>
+    <col min="15" max="15" customWidth="1" width="10"/>
+    <col min="16" max="16" customWidth="1" width="8"/>
+    <col min="17" max="17" customWidth="1" width="10"/>
+    <col min="18" max="18" customWidth="1" width="7"/>
+    <col min="19" max="19" customWidth="1" width="8"/>
+    <col min="20" max="20" customWidth="1" width="14"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="str">
+    <row r="1" ht="27.95" customHeight="1">
+      <c r="A1" s="5" t="str">
         <v>Invoice Date  *</v>
       </c>
-      <c r="B1" s="2" t="str">
+      <c r="B1" s="5" t="str">
         <v>Invoice No.  *</v>
       </c>
-      <c r="C1" s="2" t="str">
+      <c r="C1" s="6" t="str">
         <v>Billing Name</v>
       </c>
-      <c r="D1" s="2" t="str">
+      <c r="D1" s="6" t="str">
         <v>Billing GSTIN</v>
       </c>
-      <c r="E1" s="2" t="str">
+      <c r="E1" s="5" t="str">
         <v>Place of Supply  *</v>
       </c>
-      <c r="F1" s="2" t="str">
+      <c r="F1" s="6" t="str">
         <v>P/S</v>
       </c>
-      <c r="G1" s="2" t="str">
+      <c r="G1" s="6" t="str">
         <v>Item Description</v>
       </c>
-      <c r="H1" s="2" t="str">
+      <c r="H1" s="6" t="str">
         <v>HSN Code</v>
       </c>
-      <c r="I1" s="2" t="str">
+      <c r="I1" s="6" t="str">
         <v>Qty</v>
       </c>
-      <c r="J1" s="2" t="str">
+      <c r="J1" s="6" t="str">
         <v>Unit</v>
       </c>
-      <c r="K1" s="2" t="str">
+      <c r="K1" s="5" t="str">
         <v>Taxable Value  *</v>
       </c>
-      <c r="L1" s="2" t="str">
+      <c r="L1" s="6" t="str">
         <v>CGST %</v>
       </c>
-      <c r="M1" s="2" t="str">
+      <c r="M1" s="3" t="str">
         <v>CGST Amt</v>
       </c>
-      <c r="N1" s="2" t="str">
+      <c r="N1" s="6" t="str">
         <v>SGST %</v>
       </c>
-      <c r="O1" s="2" t="str">
+      <c r="O1" s="3" t="str">
         <v>SGST Amt</v>
       </c>
-      <c r="P1" s="2" t="str">
+      <c r="P1" s="6" t="str">
         <v>IGST %</v>
       </c>
-      <c r="Q1" s="2" t="str">
+      <c r="Q1" s="3" t="str">
         <v>IGST Amt</v>
       </c>
-      <c r="R1" s="2" t="str">
+      <c r="R1" s="6" t="str">
         <v>Rev Chg</v>
       </c>
-      <c r="S1" s="2" t="str">
+      <c r="S1" s="6" t="str">
         <v>Rate %</v>
       </c>
-      <c r="T1" s="2" t="str">
+      <c r="T1" s="5" t="str">
         <v>Total Value  *</v>
       </c>
     </row>
@@ -596,473 +568,1977 @@
       </c>
     </row>
     <row r="7">
+      <c r="M7" s="4" t="str">
+        <f>IF(K7="","",ROUND(K7*L7/100,2))</f>
+        <v/>
+      </c>
       <c r="N7" s="2">
         <f>L7</f>
       </c>
+      <c r="O7" s="4" t="str">
+        <f>IF(K7="","",ROUND(K7*N7/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q7" s="4" t="str">
+        <f>IF(K7="","",ROUND(K7*P7/100,2))</f>
+        <v/>
+      </c>
+      <c r="T7" s="4" t="str">
+        <f>IF(K7="","",ROUND(K7+M7+O7+Q7,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="8">
+      <c r="M8" s="4" t="str">
+        <f>IF(K8="","",ROUND(K8*L8/100,2))</f>
+        <v/>
+      </c>
       <c r="N8" s="2">
         <f>L8</f>
       </c>
+      <c r="O8" s="4" t="str">
+        <f>IF(K8="","",ROUND(K8*N8/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q8" s="4" t="str">
+        <f>IF(K8="","",ROUND(K8*P8/100,2))</f>
+        <v/>
+      </c>
+      <c r="T8" s="4" t="str">
+        <f>IF(K8="","",ROUND(K8+M8+O8+Q8,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="9">
+      <c r="M9" s="4" t="str">
+        <f>IF(K9="","",ROUND(K9*L9/100,2))</f>
+        <v/>
+      </c>
       <c r="N9" s="2">
         <f>L9</f>
       </c>
+      <c r="O9" s="4" t="str">
+        <f>IF(K9="","",ROUND(K9*N9/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q9" s="4" t="str">
+        <f>IF(K9="","",ROUND(K9*P9/100,2))</f>
+        <v/>
+      </c>
+      <c r="T9" s="4" t="str">
+        <f>IF(K9="","",ROUND(K9+M9+O9+Q9,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="10">
+      <c r="M10" s="4" t="str">
+        <f>IF(K10="","",ROUND(K10*L10/100,2))</f>
+        <v/>
+      </c>
       <c r="N10" s="2">
         <f>L10</f>
       </c>
+      <c r="O10" s="4" t="str">
+        <f>IF(K10="","",ROUND(K10*N10/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q10" s="4" t="str">
+        <f>IF(K10="","",ROUND(K10*P10/100,2))</f>
+        <v/>
+      </c>
+      <c r="T10" s="4" t="str">
+        <f>IF(K10="","",ROUND(K10+M10+O10+Q10,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="11">
+      <c r="M11" s="4" t="str">
+        <f>IF(K11="","",ROUND(K11*L11/100,2))</f>
+        <v/>
+      </c>
       <c r="N11" s="2">
         <f>L11</f>
       </c>
+      <c r="O11" s="4" t="str">
+        <f>IF(K11="","",ROUND(K11*N11/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q11" s="4" t="str">
+        <f>IF(K11="","",ROUND(K11*P11/100,2))</f>
+        <v/>
+      </c>
+      <c r="T11" s="4" t="str">
+        <f>IF(K11="","",ROUND(K11+M11+O11+Q11,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="12">
+      <c r="M12" s="4" t="str">
+        <f>IF(K12="","",ROUND(K12*L12/100,2))</f>
+        <v/>
+      </c>
       <c r="N12" s="2">
         <f>L12</f>
       </c>
+      <c r="O12" s="4" t="str">
+        <f>IF(K12="","",ROUND(K12*N12/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q12" s="4" t="str">
+        <f>IF(K12="","",ROUND(K12*P12/100,2))</f>
+        <v/>
+      </c>
+      <c r="T12" s="4" t="str">
+        <f>IF(K12="","",ROUND(K12+M12+O12+Q12,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="13">
+      <c r="M13" s="4" t="str">
+        <f>IF(K13="","",ROUND(K13*L13/100,2))</f>
+        <v/>
+      </c>
       <c r="N13" s="2">
         <f>L13</f>
       </c>
+      <c r="O13" s="4" t="str">
+        <f>IF(K13="","",ROUND(K13*N13/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q13" s="4" t="str">
+        <f>IF(K13="","",ROUND(K13*P13/100,2))</f>
+        <v/>
+      </c>
+      <c r="T13" s="4" t="str">
+        <f>IF(K13="","",ROUND(K13+M13+O13+Q13,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="14">
+      <c r="M14" s="4" t="str">
+        <f>IF(K14="","",ROUND(K14*L14/100,2))</f>
+        <v/>
+      </c>
       <c r="N14" s="2">
         <f>L14</f>
       </c>
+      <c r="O14" s="4" t="str">
+        <f>IF(K14="","",ROUND(K14*N14/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q14" s="4" t="str">
+        <f>IF(K14="","",ROUND(K14*P14/100,2))</f>
+        <v/>
+      </c>
+      <c r="T14" s="4" t="str">
+        <f>IF(K14="","",ROUND(K14+M14+O14+Q14,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="15">
+      <c r="M15" s="4" t="str">
+        <f>IF(K15="","",ROUND(K15*L15/100,2))</f>
+        <v/>
+      </c>
       <c r="N15" s="2">
         <f>L15</f>
       </c>
+      <c r="O15" s="4" t="str">
+        <f>IF(K15="","",ROUND(K15*N15/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q15" s="4" t="str">
+        <f>IF(K15="","",ROUND(K15*P15/100,2))</f>
+        <v/>
+      </c>
+      <c r="T15" s="4" t="str">
+        <f>IF(K15="","",ROUND(K15+M15+O15+Q15,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="16">
+      <c r="M16" s="4" t="str">
+        <f>IF(K16="","",ROUND(K16*L16/100,2))</f>
+        <v/>
+      </c>
       <c r="N16" s="2">
         <f>L16</f>
       </c>
+      <c r="O16" s="4" t="str">
+        <f>IF(K16="","",ROUND(K16*N16/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q16" s="4" t="str">
+        <f>IF(K16="","",ROUND(K16*P16/100,2))</f>
+        <v/>
+      </c>
+      <c r="T16" s="4" t="str">
+        <f>IF(K16="","",ROUND(K16+M16+O16+Q16,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="17">
+      <c r="M17" s="4" t="str">
+        <f>IF(K17="","",ROUND(K17*L17/100,2))</f>
+        <v/>
+      </c>
       <c r="N17" s="2">
         <f>L17</f>
       </c>
+      <c r="O17" s="4" t="str">
+        <f>IF(K17="","",ROUND(K17*N17/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q17" s="4" t="str">
+        <f>IF(K17="","",ROUND(K17*P17/100,2))</f>
+        <v/>
+      </c>
+      <c r="T17" s="4" t="str">
+        <f>IF(K17="","",ROUND(K17+M17+O17+Q17,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="18">
+      <c r="M18" s="4" t="str">
+        <f>IF(K18="","",ROUND(K18*L18/100,2))</f>
+        <v/>
+      </c>
       <c r="N18" s="2">
         <f>L18</f>
       </c>
+      <c r="O18" s="4" t="str">
+        <f>IF(K18="","",ROUND(K18*N18/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q18" s="4" t="str">
+        <f>IF(K18="","",ROUND(K18*P18/100,2))</f>
+        <v/>
+      </c>
+      <c r="T18" s="4" t="str">
+        <f>IF(K18="","",ROUND(K18+M18+O18+Q18,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="19">
+      <c r="M19" s="4" t="str">
+        <f>IF(K19="","",ROUND(K19*L19/100,2))</f>
+        <v/>
+      </c>
       <c r="N19" s="2">
         <f>L19</f>
       </c>
+      <c r="O19" s="4" t="str">
+        <f>IF(K19="","",ROUND(K19*N19/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q19" s="4" t="str">
+        <f>IF(K19="","",ROUND(K19*P19/100,2))</f>
+        <v/>
+      </c>
+      <c r="T19" s="4" t="str">
+        <f>IF(K19="","",ROUND(K19+M19+O19+Q19,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="20">
+      <c r="M20" s="4" t="str">
+        <f>IF(K20="","",ROUND(K20*L20/100,2))</f>
+        <v/>
+      </c>
       <c r="N20" s="2">
         <f>L20</f>
       </c>
+      <c r="O20" s="4" t="str">
+        <f>IF(K20="","",ROUND(K20*N20/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q20" s="4" t="str">
+        <f>IF(K20="","",ROUND(K20*P20/100,2))</f>
+        <v/>
+      </c>
+      <c r="T20" s="4" t="str">
+        <f>IF(K20="","",ROUND(K20+M20+O20+Q20,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="21">
+      <c r="M21" s="4" t="str">
+        <f>IF(K21="","",ROUND(K21*L21/100,2))</f>
+        <v/>
+      </c>
       <c r="N21" s="2">
         <f>L21</f>
       </c>
+      <c r="O21" s="4" t="str">
+        <f>IF(K21="","",ROUND(K21*N21/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q21" s="4" t="str">
+        <f>IF(K21="","",ROUND(K21*P21/100,2))</f>
+        <v/>
+      </c>
+      <c r="T21" s="4" t="str">
+        <f>IF(K21="","",ROUND(K21+M21+O21+Q21,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="22">
+      <c r="M22" s="4" t="str">
+        <f>IF(K22="","",ROUND(K22*L22/100,2))</f>
+        <v/>
+      </c>
       <c r="N22" s="2">
         <f>L22</f>
       </c>
+      <c r="O22" s="4" t="str">
+        <f>IF(K22="","",ROUND(K22*N22/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q22" s="4" t="str">
+        <f>IF(K22="","",ROUND(K22*P22/100,2))</f>
+        <v/>
+      </c>
+      <c r="T22" s="4" t="str">
+        <f>IF(K22="","",ROUND(K22+M22+O22+Q22,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="23">
+      <c r="M23" s="4" t="str">
+        <f>IF(K23="","",ROUND(K23*L23/100,2))</f>
+        <v/>
+      </c>
       <c r="N23" s="2">
         <f>L23</f>
       </c>
+      <c r="O23" s="4" t="str">
+        <f>IF(K23="","",ROUND(K23*N23/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q23" s="4" t="str">
+        <f>IF(K23="","",ROUND(K23*P23/100,2))</f>
+        <v/>
+      </c>
+      <c r="T23" s="4" t="str">
+        <f>IF(K23="","",ROUND(K23+M23+O23+Q23,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="24">
+      <c r="M24" s="4" t="str">
+        <f>IF(K24="","",ROUND(K24*L24/100,2))</f>
+        <v/>
+      </c>
       <c r="N24" s="2">
         <f>L24</f>
       </c>
+      <c r="O24" s="4" t="str">
+        <f>IF(K24="","",ROUND(K24*N24/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q24" s="4" t="str">
+        <f>IF(K24="","",ROUND(K24*P24/100,2))</f>
+        <v/>
+      </c>
+      <c r="T24" s="4" t="str">
+        <f>IF(K24="","",ROUND(K24+M24+O24+Q24,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="25">
+      <c r="M25" s="4" t="str">
+        <f>IF(K25="","",ROUND(K25*L25/100,2))</f>
+        <v/>
+      </c>
       <c r="N25" s="2">
         <f>L25</f>
       </c>
+      <c r="O25" s="4" t="str">
+        <f>IF(K25="","",ROUND(K25*N25/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q25" s="4" t="str">
+        <f>IF(K25="","",ROUND(K25*P25/100,2))</f>
+        <v/>
+      </c>
+      <c r="T25" s="4" t="str">
+        <f>IF(K25="","",ROUND(K25+M25+O25+Q25,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="26">
+      <c r="M26" s="4" t="str">
+        <f>IF(K26="","",ROUND(K26*L26/100,2))</f>
+        <v/>
+      </c>
       <c r="N26" s="2">
         <f>L26</f>
       </c>
+      <c r="O26" s="4" t="str">
+        <f>IF(K26="","",ROUND(K26*N26/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q26" s="4" t="str">
+        <f>IF(K26="","",ROUND(K26*P26/100,2))</f>
+        <v/>
+      </c>
+      <c r="T26" s="4" t="str">
+        <f>IF(K26="","",ROUND(K26+M26+O26+Q26,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="27">
+      <c r="M27" s="4" t="str">
+        <f>IF(K27="","",ROUND(K27*L27/100,2))</f>
+        <v/>
+      </c>
       <c r="N27" s="2">
         <f>L27</f>
       </c>
+      <c r="O27" s="4" t="str">
+        <f>IF(K27="","",ROUND(K27*N27/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q27" s="4" t="str">
+        <f>IF(K27="","",ROUND(K27*P27/100,2))</f>
+        <v/>
+      </c>
+      <c r="T27" s="4" t="str">
+        <f>IF(K27="","",ROUND(K27+M27+O27+Q27,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="28">
+      <c r="M28" s="4" t="str">
+        <f>IF(K28="","",ROUND(K28*L28/100,2))</f>
+        <v/>
+      </c>
       <c r="N28" s="2">
         <f>L28</f>
       </c>
+      <c r="O28" s="4" t="str">
+        <f>IF(K28="","",ROUND(K28*N28/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q28" s="4" t="str">
+        <f>IF(K28="","",ROUND(K28*P28/100,2))</f>
+        <v/>
+      </c>
+      <c r="T28" s="4" t="str">
+        <f>IF(K28="","",ROUND(K28+M28+O28+Q28,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="29">
+      <c r="M29" s="4" t="str">
+        <f>IF(K29="","",ROUND(K29*L29/100,2))</f>
+        <v/>
+      </c>
       <c r="N29" s="2">
         <f>L29</f>
       </c>
+      <c r="O29" s="4" t="str">
+        <f>IF(K29="","",ROUND(K29*N29/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q29" s="4" t="str">
+        <f>IF(K29="","",ROUND(K29*P29/100,2))</f>
+        <v/>
+      </c>
+      <c r="T29" s="4" t="str">
+        <f>IF(K29="","",ROUND(K29+M29+O29+Q29,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="30">
+      <c r="M30" s="4" t="str">
+        <f>IF(K30="","",ROUND(K30*L30/100,2))</f>
+        <v/>
+      </c>
       <c r="N30" s="2">
         <f>L30</f>
       </c>
+      <c r="O30" s="4" t="str">
+        <f>IF(K30="","",ROUND(K30*N30/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q30" s="4" t="str">
+        <f>IF(K30="","",ROUND(K30*P30/100,2))</f>
+        <v/>
+      </c>
+      <c r="T30" s="4" t="str">
+        <f>IF(K30="","",ROUND(K30+M30+O30+Q30,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="31">
+      <c r="M31" s="4" t="str">
+        <f>IF(K31="","",ROUND(K31*L31/100,2))</f>
+        <v/>
+      </c>
       <c r="N31" s="2">
         <f>L31</f>
       </c>
+      <c r="O31" s="4" t="str">
+        <f>IF(K31="","",ROUND(K31*N31/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q31" s="4" t="str">
+        <f>IF(K31="","",ROUND(K31*P31/100,2))</f>
+        <v/>
+      </c>
+      <c r="T31" s="4" t="str">
+        <f>IF(K31="","",ROUND(K31+M31+O31+Q31,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="32">
+      <c r="M32" s="4" t="str">
+        <f>IF(K32="","",ROUND(K32*L32/100,2))</f>
+        <v/>
+      </c>
       <c r="N32" s="2">
         <f>L32</f>
       </c>
+      <c r="O32" s="4" t="str">
+        <f>IF(K32="","",ROUND(K32*N32/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q32" s="4" t="str">
+        <f>IF(K32="","",ROUND(K32*P32/100,2))</f>
+        <v/>
+      </c>
+      <c r="T32" s="4" t="str">
+        <f>IF(K32="","",ROUND(K32+M32+O32+Q32,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="33">
+      <c r="M33" s="4" t="str">
+        <f>IF(K33="","",ROUND(K33*L33/100,2))</f>
+        <v/>
+      </c>
       <c r="N33" s="2">
         <f>L33</f>
       </c>
+      <c r="O33" s="4" t="str">
+        <f>IF(K33="","",ROUND(K33*N33/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q33" s="4" t="str">
+        <f>IF(K33="","",ROUND(K33*P33/100,2))</f>
+        <v/>
+      </c>
+      <c r="T33" s="4" t="str">
+        <f>IF(K33="","",ROUND(K33+M33+O33+Q33,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="34">
+      <c r="M34" s="4" t="str">
+        <f>IF(K34="","",ROUND(K34*L34/100,2))</f>
+        <v/>
+      </c>
       <c r="N34" s="2">
         <f>L34</f>
       </c>
+      <c r="O34" s="4" t="str">
+        <f>IF(K34="","",ROUND(K34*N34/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q34" s="4" t="str">
+        <f>IF(K34="","",ROUND(K34*P34/100,2))</f>
+        <v/>
+      </c>
+      <c r="T34" s="4" t="str">
+        <f>IF(K34="","",ROUND(K34+M34+O34+Q34,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="35">
+      <c r="M35" s="4" t="str">
+        <f>IF(K35="","",ROUND(K35*L35/100,2))</f>
+        <v/>
+      </c>
       <c r="N35" s="2">
         <f>L35</f>
       </c>
+      <c r="O35" s="4" t="str">
+        <f>IF(K35="","",ROUND(K35*N35/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q35" s="4" t="str">
+        <f>IF(K35="","",ROUND(K35*P35/100,2))</f>
+        <v/>
+      </c>
+      <c r="T35" s="4" t="str">
+        <f>IF(K35="","",ROUND(K35+M35+O35+Q35,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="36">
+      <c r="M36" s="4" t="str">
+        <f>IF(K36="","",ROUND(K36*L36/100,2))</f>
+        <v/>
+      </c>
       <c r="N36" s="2">
         <f>L36</f>
       </c>
+      <c r="O36" s="4" t="str">
+        <f>IF(K36="","",ROUND(K36*N36/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q36" s="4" t="str">
+        <f>IF(K36="","",ROUND(K36*P36/100,2))</f>
+        <v/>
+      </c>
+      <c r="T36" s="4" t="str">
+        <f>IF(K36="","",ROUND(K36+M36+O36+Q36,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="37">
+      <c r="M37" s="4" t="str">
+        <f>IF(K37="","",ROUND(K37*L37/100,2))</f>
+        <v/>
+      </c>
       <c r="N37" s="2">
         <f>L37</f>
       </c>
+      <c r="O37" s="4" t="str">
+        <f>IF(K37="","",ROUND(K37*N37/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q37" s="4" t="str">
+        <f>IF(K37="","",ROUND(K37*P37/100,2))</f>
+        <v/>
+      </c>
+      <c r="T37" s="4" t="str">
+        <f>IF(K37="","",ROUND(K37+M37+O37+Q37,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="38">
+      <c r="M38" s="4" t="str">
+        <f>IF(K38="","",ROUND(K38*L38/100,2))</f>
+        <v/>
+      </c>
       <c r="N38" s="2">
         <f>L38</f>
       </c>
+      <c r="O38" s="4" t="str">
+        <f>IF(K38="","",ROUND(K38*N38/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q38" s="4" t="str">
+        <f>IF(K38="","",ROUND(K38*P38/100,2))</f>
+        <v/>
+      </c>
+      <c r="T38" s="4" t="str">
+        <f>IF(K38="","",ROUND(K38+M38+O38+Q38,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="39">
+      <c r="M39" s="4" t="str">
+        <f>IF(K39="","",ROUND(K39*L39/100,2))</f>
+        <v/>
+      </c>
       <c r="N39" s="2">
         <f>L39</f>
       </c>
+      <c r="O39" s="4" t="str">
+        <f>IF(K39="","",ROUND(K39*N39/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q39" s="4" t="str">
+        <f>IF(K39="","",ROUND(K39*P39/100,2))</f>
+        <v/>
+      </c>
+      <c r="T39" s="4" t="str">
+        <f>IF(K39="","",ROUND(K39+M39+O39+Q39,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="40">
+      <c r="M40" s="4" t="str">
+        <f>IF(K40="","",ROUND(K40*L40/100,2))</f>
+        <v/>
+      </c>
       <c r="N40" s="2">
         <f>L40</f>
       </c>
+      <c r="O40" s="4" t="str">
+        <f>IF(K40="","",ROUND(K40*N40/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q40" s="4" t="str">
+        <f>IF(K40="","",ROUND(K40*P40/100,2))</f>
+        <v/>
+      </c>
+      <c r="T40" s="4" t="str">
+        <f>IF(K40="","",ROUND(K40+M40+O40+Q40,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="41">
+      <c r="M41" s="4" t="str">
+        <f>IF(K41="","",ROUND(K41*L41/100,2))</f>
+        <v/>
+      </c>
       <c r="N41" s="2">
         <f>L41</f>
       </c>
+      <c r="O41" s="4" t="str">
+        <f>IF(K41="","",ROUND(K41*N41/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q41" s="4" t="str">
+        <f>IF(K41="","",ROUND(K41*P41/100,2))</f>
+        <v/>
+      </c>
+      <c r="T41" s="4" t="str">
+        <f>IF(K41="","",ROUND(K41+M41+O41+Q41,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="42">
+      <c r="M42" s="4" t="str">
+        <f>IF(K42="","",ROUND(K42*L42/100,2))</f>
+        <v/>
+      </c>
       <c r="N42" s="2">
         <f>L42</f>
       </c>
+      <c r="O42" s="4" t="str">
+        <f>IF(K42="","",ROUND(K42*N42/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q42" s="4" t="str">
+        <f>IF(K42="","",ROUND(K42*P42/100,2))</f>
+        <v/>
+      </c>
+      <c r="T42" s="4" t="str">
+        <f>IF(K42="","",ROUND(K42+M42+O42+Q42,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="43">
+      <c r="M43" s="4" t="str">
+        <f>IF(K43="","",ROUND(K43*L43/100,2))</f>
+        <v/>
+      </c>
       <c r="N43" s="2">
         <f>L43</f>
       </c>
+      <c r="O43" s="4" t="str">
+        <f>IF(K43="","",ROUND(K43*N43/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q43" s="4" t="str">
+        <f>IF(K43="","",ROUND(K43*P43/100,2))</f>
+        <v/>
+      </c>
+      <c r="T43" s="4" t="str">
+        <f>IF(K43="","",ROUND(K43+M43+O43+Q43,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="44">
+      <c r="M44" s="4" t="str">
+        <f>IF(K44="","",ROUND(K44*L44/100,2))</f>
+        <v/>
+      </c>
       <c r="N44" s="2">
         <f>L44</f>
       </c>
+      <c r="O44" s="4" t="str">
+        <f>IF(K44="","",ROUND(K44*N44/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q44" s="4" t="str">
+        <f>IF(K44="","",ROUND(K44*P44/100,2))</f>
+        <v/>
+      </c>
+      <c r="T44" s="4" t="str">
+        <f>IF(K44="","",ROUND(K44+M44+O44+Q44,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="45">
+      <c r="M45" s="4" t="str">
+        <f>IF(K45="","",ROUND(K45*L45/100,2))</f>
+        <v/>
+      </c>
       <c r="N45" s="2">
         <f>L45</f>
       </c>
+      <c r="O45" s="4" t="str">
+        <f>IF(K45="","",ROUND(K45*N45/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q45" s="4" t="str">
+        <f>IF(K45="","",ROUND(K45*P45/100,2))</f>
+        <v/>
+      </c>
+      <c r="T45" s="4" t="str">
+        <f>IF(K45="","",ROUND(K45+M45+O45+Q45,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="46">
+      <c r="M46" s="4" t="str">
+        <f>IF(K46="","",ROUND(K46*L46/100,2))</f>
+        <v/>
+      </c>
       <c r="N46" s="2">
         <f>L46</f>
       </c>
+      <c r="O46" s="4" t="str">
+        <f>IF(K46="","",ROUND(K46*N46/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q46" s="4" t="str">
+        <f>IF(K46="","",ROUND(K46*P46/100,2))</f>
+        <v/>
+      </c>
+      <c r="T46" s="4" t="str">
+        <f>IF(K46="","",ROUND(K46+M46+O46+Q46,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="47">
+      <c r="M47" s="4" t="str">
+        <f>IF(K47="","",ROUND(K47*L47/100,2))</f>
+        <v/>
+      </c>
       <c r="N47" s="2">
         <f>L47</f>
       </c>
+      <c r="O47" s="4" t="str">
+        <f>IF(K47="","",ROUND(K47*N47/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q47" s="4" t="str">
+        <f>IF(K47="","",ROUND(K47*P47/100,2))</f>
+        <v/>
+      </c>
+      <c r="T47" s="4" t="str">
+        <f>IF(K47="","",ROUND(K47+M47+O47+Q47,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="48">
+      <c r="M48" s="4" t="str">
+        <f>IF(K48="","",ROUND(K48*L48/100,2))</f>
+        <v/>
+      </c>
       <c r="N48" s="2">
         <f>L48</f>
       </c>
+      <c r="O48" s="4" t="str">
+        <f>IF(K48="","",ROUND(K48*N48/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q48" s="4" t="str">
+        <f>IF(K48="","",ROUND(K48*P48/100,2))</f>
+        <v/>
+      </c>
+      <c r="T48" s="4" t="str">
+        <f>IF(K48="","",ROUND(K48+M48+O48+Q48,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="49">
+      <c r="M49" s="4" t="str">
+        <f>IF(K49="","",ROUND(K49*L49/100,2))</f>
+        <v/>
+      </c>
       <c r="N49" s="2">
         <f>L49</f>
       </c>
+      <c r="O49" s="4" t="str">
+        <f>IF(K49="","",ROUND(K49*N49/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q49" s="4" t="str">
+        <f>IF(K49="","",ROUND(K49*P49/100,2))</f>
+        <v/>
+      </c>
+      <c r="T49" s="4" t="str">
+        <f>IF(K49="","",ROUND(K49+M49+O49+Q49,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="50">
+      <c r="M50" s="4" t="str">
+        <f>IF(K50="","",ROUND(K50*L50/100,2))</f>
+        <v/>
+      </c>
       <c r="N50" s="2">
         <f>L50</f>
       </c>
+      <c r="O50" s="4" t="str">
+        <f>IF(K50="","",ROUND(K50*N50/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q50" s="4" t="str">
+        <f>IF(K50="","",ROUND(K50*P50/100,2))</f>
+        <v/>
+      </c>
+      <c r="T50" s="4" t="str">
+        <f>IF(K50="","",ROUND(K50+M50+O50+Q50,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="51">
+      <c r="M51" s="4" t="str">
+        <f>IF(K51="","",ROUND(K51*L51/100,2))</f>
+        <v/>
+      </c>
       <c r="N51" s="2">
         <f>L51</f>
       </c>
+      <c r="O51" s="4" t="str">
+        <f>IF(K51="","",ROUND(K51*N51/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q51" s="4" t="str">
+        <f>IF(K51="","",ROUND(K51*P51/100,2))</f>
+        <v/>
+      </c>
+      <c r="T51" s="4" t="str">
+        <f>IF(K51="","",ROUND(K51+M51+O51+Q51,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="52">
+      <c r="M52" s="4" t="str">
+        <f>IF(K52="","",ROUND(K52*L52/100,2))</f>
+        <v/>
+      </c>
       <c r="N52" s="2">
         <f>L52</f>
       </c>
+      <c r="O52" s="4" t="str">
+        <f>IF(K52="","",ROUND(K52*N52/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q52" s="4" t="str">
+        <f>IF(K52="","",ROUND(K52*P52/100,2))</f>
+        <v/>
+      </c>
+      <c r="T52" s="4" t="str">
+        <f>IF(K52="","",ROUND(K52+M52+O52+Q52,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="53">
+      <c r="M53" s="4" t="str">
+        <f>IF(K53="","",ROUND(K53*L53/100,2))</f>
+        <v/>
+      </c>
       <c r="N53" s="2">
         <f>L53</f>
       </c>
+      <c r="O53" s="4" t="str">
+        <f>IF(K53="","",ROUND(K53*N53/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q53" s="4" t="str">
+        <f>IF(K53="","",ROUND(K53*P53/100,2))</f>
+        <v/>
+      </c>
+      <c r="T53" s="4" t="str">
+        <f>IF(K53="","",ROUND(K53+M53+O53+Q53,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="54">
+      <c r="M54" s="4" t="str">
+        <f>IF(K54="","",ROUND(K54*L54/100,2))</f>
+        <v/>
+      </c>
       <c r="N54" s="2">
         <f>L54</f>
       </c>
+      <c r="O54" s="4" t="str">
+        <f>IF(K54="","",ROUND(K54*N54/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q54" s="4" t="str">
+        <f>IF(K54="","",ROUND(K54*P54/100,2))</f>
+        <v/>
+      </c>
+      <c r="T54" s="4" t="str">
+        <f>IF(K54="","",ROUND(K54+M54+O54+Q54,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="55">
+      <c r="M55" s="4" t="str">
+        <f>IF(K55="","",ROUND(K55*L55/100,2))</f>
+        <v/>
+      </c>
       <c r="N55" s="2">
         <f>L55</f>
       </c>
+      <c r="O55" s="4" t="str">
+        <f>IF(K55="","",ROUND(K55*N55/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q55" s="4" t="str">
+        <f>IF(K55="","",ROUND(K55*P55/100,2))</f>
+        <v/>
+      </c>
+      <c r="T55" s="4" t="str">
+        <f>IF(K55="","",ROUND(K55+M55+O55+Q55,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="56">
+      <c r="M56" s="4" t="str">
+        <f>IF(K56="","",ROUND(K56*L56/100,2))</f>
+        <v/>
+      </c>
       <c r="N56" s="2">
         <f>L56</f>
       </c>
+      <c r="O56" s="4" t="str">
+        <f>IF(K56="","",ROUND(K56*N56/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q56" s="4" t="str">
+        <f>IF(K56="","",ROUND(K56*P56/100,2))</f>
+        <v/>
+      </c>
+      <c r="T56" s="4" t="str">
+        <f>IF(K56="","",ROUND(K56+M56+O56+Q56,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="57">
+      <c r="M57" s="4" t="str">
+        <f>IF(K57="","",ROUND(K57*L57/100,2))</f>
+        <v/>
+      </c>
       <c r="N57" s="2">
         <f>L57</f>
       </c>
+      <c r="O57" s="4" t="str">
+        <f>IF(K57="","",ROUND(K57*N57/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q57" s="4" t="str">
+        <f>IF(K57="","",ROUND(K57*P57/100,2))</f>
+        <v/>
+      </c>
+      <c r="T57" s="4" t="str">
+        <f>IF(K57="","",ROUND(K57+M57+O57+Q57,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="58">
+      <c r="M58" s="4" t="str">
+        <f>IF(K58="","",ROUND(K58*L58/100,2))</f>
+        <v/>
+      </c>
       <c r="N58" s="2">
         <f>L58</f>
       </c>
+      <c r="O58" s="4" t="str">
+        <f>IF(K58="","",ROUND(K58*N58/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q58" s="4" t="str">
+        <f>IF(K58="","",ROUND(K58*P58/100,2))</f>
+        <v/>
+      </c>
+      <c r="T58" s="4" t="str">
+        <f>IF(K58="","",ROUND(K58+M58+O58+Q58,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="59">
+      <c r="M59" s="4" t="str">
+        <f>IF(K59="","",ROUND(K59*L59/100,2))</f>
+        <v/>
+      </c>
       <c r="N59" s="2">
         <f>L59</f>
       </c>
+      <c r="O59" s="4" t="str">
+        <f>IF(K59="","",ROUND(K59*N59/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q59" s="4" t="str">
+        <f>IF(K59="","",ROUND(K59*P59/100,2))</f>
+        <v/>
+      </c>
+      <c r="T59" s="4" t="str">
+        <f>IF(K59="","",ROUND(K59+M59+O59+Q59,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="60">
+      <c r="M60" s="4" t="str">
+        <f>IF(K60="","",ROUND(K60*L60/100,2))</f>
+        <v/>
+      </c>
       <c r="N60" s="2">
         <f>L60</f>
       </c>
+      <c r="O60" s="4" t="str">
+        <f>IF(K60="","",ROUND(K60*N60/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q60" s="4" t="str">
+        <f>IF(K60="","",ROUND(K60*P60/100,2))</f>
+        <v/>
+      </c>
+      <c r="T60" s="4" t="str">
+        <f>IF(K60="","",ROUND(K60+M60+O60+Q60,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="61">
+      <c r="M61" s="4" t="str">
+        <f>IF(K61="","",ROUND(K61*L61/100,2))</f>
+        <v/>
+      </c>
       <c r="N61" s="2">
         <f>L61</f>
       </c>
+      <c r="O61" s="4" t="str">
+        <f>IF(K61="","",ROUND(K61*N61/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q61" s="4" t="str">
+        <f>IF(K61="","",ROUND(K61*P61/100,2))</f>
+        <v/>
+      </c>
+      <c r="T61" s="4" t="str">
+        <f>IF(K61="","",ROUND(K61+M61+O61+Q61,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="62">
+      <c r="M62" s="4" t="str">
+        <f>IF(K62="","",ROUND(K62*L62/100,2))</f>
+        <v/>
+      </c>
       <c r="N62" s="2">
         <f>L62</f>
       </c>
+      <c r="O62" s="4" t="str">
+        <f>IF(K62="","",ROUND(K62*N62/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q62" s="4" t="str">
+        <f>IF(K62="","",ROUND(K62*P62/100,2))</f>
+        <v/>
+      </c>
+      <c r="T62" s="4" t="str">
+        <f>IF(K62="","",ROUND(K62+M62+O62+Q62,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="63">
+      <c r="M63" s="4" t="str">
+        <f>IF(K63="","",ROUND(K63*L63/100,2))</f>
+        <v/>
+      </c>
       <c r="N63" s="2">
         <f>L63</f>
       </c>
+      <c r="O63" s="4" t="str">
+        <f>IF(K63="","",ROUND(K63*N63/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q63" s="4" t="str">
+        <f>IF(K63="","",ROUND(K63*P63/100,2))</f>
+        <v/>
+      </c>
+      <c r="T63" s="4" t="str">
+        <f>IF(K63="","",ROUND(K63+M63+O63+Q63,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="64">
+      <c r="M64" s="4" t="str">
+        <f>IF(K64="","",ROUND(K64*L64/100,2))</f>
+        <v/>
+      </c>
       <c r="N64" s="2">
         <f>L64</f>
       </c>
+      <c r="O64" s="4" t="str">
+        <f>IF(K64="","",ROUND(K64*N64/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q64" s="4" t="str">
+        <f>IF(K64="","",ROUND(K64*P64/100,2))</f>
+        <v/>
+      </c>
+      <c r="T64" s="4" t="str">
+        <f>IF(K64="","",ROUND(K64+M64+O64+Q64,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="65">
+      <c r="M65" s="4" t="str">
+        <f>IF(K65="","",ROUND(K65*L65/100,2))</f>
+        <v/>
+      </c>
       <c r="N65" s="2">
         <f>L65</f>
       </c>
+      <c r="O65" s="4" t="str">
+        <f>IF(K65="","",ROUND(K65*N65/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q65" s="4" t="str">
+        <f>IF(K65="","",ROUND(K65*P65/100,2))</f>
+        <v/>
+      </c>
+      <c r="T65" s="4" t="str">
+        <f>IF(K65="","",ROUND(K65+M65+O65+Q65,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="66">
+      <c r="M66" s="4" t="str">
+        <f>IF(K66="","",ROUND(K66*L66/100,2))</f>
+        <v/>
+      </c>
       <c r="N66" s="2">
         <f>L66</f>
       </c>
+      <c r="O66" s="4" t="str">
+        <f>IF(K66="","",ROUND(K66*N66/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q66" s="4" t="str">
+        <f>IF(K66="","",ROUND(K66*P66/100,2))</f>
+        <v/>
+      </c>
+      <c r="T66" s="4" t="str">
+        <f>IF(K66="","",ROUND(K66+M66+O66+Q66,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="67">
+      <c r="M67" s="4" t="str">
+        <f>IF(K67="","",ROUND(K67*L67/100,2))</f>
+        <v/>
+      </c>
       <c r="N67" s="2">
         <f>L67</f>
       </c>
+      <c r="O67" s="4" t="str">
+        <f>IF(K67="","",ROUND(K67*N67/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q67" s="4" t="str">
+        <f>IF(K67="","",ROUND(K67*P67/100,2))</f>
+        <v/>
+      </c>
+      <c r="T67" s="4" t="str">
+        <f>IF(K67="","",ROUND(K67+M67+O67+Q67,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="68">
+      <c r="M68" s="4" t="str">
+        <f>IF(K68="","",ROUND(K68*L68/100,2))</f>
+        <v/>
+      </c>
       <c r="N68" s="2">
         <f>L68</f>
       </c>
+      <c r="O68" s="4" t="str">
+        <f>IF(K68="","",ROUND(K68*N68/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q68" s="4" t="str">
+        <f>IF(K68="","",ROUND(K68*P68/100,2))</f>
+        <v/>
+      </c>
+      <c r="T68" s="4" t="str">
+        <f>IF(K68="","",ROUND(K68+M68+O68+Q68,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="69">
+      <c r="M69" s="4" t="str">
+        <f>IF(K69="","",ROUND(K69*L69/100,2))</f>
+        <v/>
+      </c>
       <c r="N69" s="2">
         <f>L69</f>
       </c>
+      <c r="O69" s="4" t="str">
+        <f>IF(K69="","",ROUND(K69*N69/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q69" s="4" t="str">
+        <f>IF(K69="","",ROUND(K69*P69/100,2))</f>
+        <v/>
+      </c>
+      <c r="T69" s="4" t="str">
+        <f>IF(K69="","",ROUND(K69+M69+O69+Q69,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="70">
+      <c r="M70" s="4" t="str">
+        <f>IF(K70="","",ROUND(K70*L70/100,2))</f>
+        <v/>
+      </c>
       <c r="N70" s="2">
         <f>L70</f>
       </c>
+      <c r="O70" s="4" t="str">
+        <f>IF(K70="","",ROUND(K70*N70/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q70" s="4" t="str">
+        <f>IF(K70="","",ROUND(K70*P70/100,2))</f>
+        <v/>
+      </c>
+      <c r="T70" s="4" t="str">
+        <f>IF(K70="","",ROUND(K70+M70+O70+Q70,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="71">
+      <c r="M71" s="4" t="str">
+        <f>IF(K71="","",ROUND(K71*L71/100,2))</f>
+        <v/>
+      </c>
       <c r="N71" s="2">
         <f>L71</f>
       </c>
+      <c r="O71" s="4" t="str">
+        <f>IF(K71="","",ROUND(K71*N71/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q71" s="4" t="str">
+        <f>IF(K71="","",ROUND(K71*P71/100,2))</f>
+        <v/>
+      </c>
+      <c r="T71" s="4" t="str">
+        <f>IF(K71="","",ROUND(K71+M71+O71+Q71,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="72">
+      <c r="M72" s="4" t="str">
+        <f>IF(K72="","",ROUND(K72*L72/100,2))</f>
+        <v/>
+      </c>
       <c r="N72" s="2">
         <f>L72</f>
       </c>
+      <c r="O72" s="4" t="str">
+        <f>IF(K72="","",ROUND(K72*N72/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q72" s="4" t="str">
+        <f>IF(K72="","",ROUND(K72*P72/100,2))</f>
+        <v/>
+      </c>
+      <c r="T72" s="4" t="str">
+        <f>IF(K72="","",ROUND(K72+M72+O72+Q72,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="73">
+      <c r="M73" s="4" t="str">
+        <f>IF(K73="","",ROUND(K73*L73/100,2))</f>
+        <v/>
+      </c>
       <c r="N73" s="2">
         <f>L73</f>
       </c>
+      <c r="O73" s="4" t="str">
+        <f>IF(K73="","",ROUND(K73*N73/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q73" s="4" t="str">
+        <f>IF(K73="","",ROUND(K73*P73/100,2))</f>
+        <v/>
+      </c>
+      <c r="T73" s="4" t="str">
+        <f>IF(K73="","",ROUND(K73+M73+O73+Q73,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="74">
+      <c r="M74" s="4" t="str">
+        <f>IF(K74="","",ROUND(K74*L74/100,2))</f>
+        <v/>
+      </c>
       <c r="N74" s="2">
         <f>L74</f>
       </c>
+      <c r="O74" s="4" t="str">
+        <f>IF(K74="","",ROUND(K74*N74/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q74" s="4" t="str">
+        <f>IF(K74="","",ROUND(K74*P74/100,2))</f>
+        <v/>
+      </c>
+      <c r="T74" s="4" t="str">
+        <f>IF(K74="","",ROUND(K74+M74+O74+Q74,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="75">
+      <c r="M75" s="4" t="str">
+        <f>IF(K75="","",ROUND(K75*L75/100,2))</f>
+        <v/>
+      </c>
       <c r="N75" s="2">
         <f>L75</f>
       </c>
+      <c r="O75" s="4" t="str">
+        <f>IF(K75="","",ROUND(K75*N75/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q75" s="4" t="str">
+        <f>IF(K75="","",ROUND(K75*P75/100,2))</f>
+        <v/>
+      </c>
+      <c r="T75" s="4" t="str">
+        <f>IF(K75="","",ROUND(K75+M75+O75+Q75,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="76">
+      <c r="M76" s="4" t="str">
+        <f>IF(K76="","",ROUND(K76*L76/100,2))</f>
+        <v/>
+      </c>
       <c r="N76" s="2">
         <f>L76</f>
       </c>
+      <c r="O76" s="4" t="str">
+        <f>IF(K76="","",ROUND(K76*N76/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q76" s="4" t="str">
+        <f>IF(K76="","",ROUND(K76*P76/100,2))</f>
+        <v/>
+      </c>
+      <c r="T76" s="4" t="str">
+        <f>IF(K76="","",ROUND(K76+M76+O76+Q76,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="77">
+      <c r="M77" s="4" t="str">
+        <f>IF(K77="","",ROUND(K77*L77/100,2))</f>
+        <v/>
+      </c>
       <c r="N77" s="2">
         <f>L77</f>
       </c>
+      <c r="O77" s="4" t="str">
+        <f>IF(K77="","",ROUND(K77*N77/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q77" s="4" t="str">
+        <f>IF(K77="","",ROUND(K77*P77/100,2))</f>
+        <v/>
+      </c>
+      <c r="T77" s="4" t="str">
+        <f>IF(K77="","",ROUND(K77+M77+O77+Q77,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="78">
+      <c r="M78" s="4" t="str">
+        <f>IF(K78="","",ROUND(K78*L78/100,2))</f>
+        <v/>
+      </c>
       <c r="N78" s="2">
         <f>L78</f>
       </c>
+      <c r="O78" s="4" t="str">
+        <f>IF(K78="","",ROUND(K78*N78/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q78" s="4" t="str">
+        <f>IF(K78="","",ROUND(K78*P78/100,2))</f>
+        <v/>
+      </c>
+      <c r="T78" s="4" t="str">
+        <f>IF(K78="","",ROUND(K78+M78+O78+Q78,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="79">
+      <c r="M79" s="4" t="str">
+        <f>IF(K79="","",ROUND(K79*L79/100,2))</f>
+        <v/>
+      </c>
       <c r="N79" s="2">
         <f>L79</f>
       </c>
+      <c r="O79" s="4" t="str">
+        <f>IF(K79="","",ROUND(K79*N79/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q79" s="4" t="str">
+        <f>IF(K79="","",ROUND(K79*P79/100,2))</f>
+        <v/>
+      </c>
+      <c r="T79" s="4" t="str">
+        <f>IF(K79="","",ROUND(K79+M79+O79+Q79,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="80">
+      <c r="M80" s="4" t="str">
+        <f>IF(K80="","",ROUND(K80*L80/100,2))</f>
+        <v/>
+      </c>
       <c r="N80" s="2">
         <f>L80</f>
       </c>
+      <c r="O80" s="4" t="str">
+        <f>IF(K80="","",ROUND(K80*N80/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q80" s="4" t="str">
+        <f>IF(K80="","",ROUND(K80*P80/100,2))</f>
+        <v/>
+      </c>
+      <c r="T80" s="4" t="str">
+        <f>IF(K80="","",ROUND(K80+M80+O80+Q80,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="81">
+      <c r="M81" s="4" t="str">
+        <f>IF(K81="","",ROUND(K81*L81/100,2))</f>
+        <v/>
+      </c>
       <c r="N81" s="2">
         <f>L81</f>
       </c>
+      <c r="O81" s="4" t="str">
+        <f>IF(K81="","",ROUND(K81*N81/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q81" s="4" t="str">
+        <f>IF(K81="","",ROUND(K81*P81/100,2))</f>
+        <v/>
+      </c>
+      <c r="T81" s="4" t="str">
+        <f>IF(K81="","",ROUND(K81+M81+O81+Q81,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="82">
+      <c r="M82" s="4" t="str">
+        <f>IF(K82="","",ROUND(K82*L82/100,2))</f>
+        <v/>
+      </c>
       <c r="N82" s="2">
         <f>L82</f>
       </c>
+      <c r="O82" s="4" t="str">
+        <f>IF(K82="","",ROUND(K82*N82/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q82" s="4" t="str">
+        <f>IF(K82="","",ROUND(K82*P82/100,2))</f>
+        <v/>
+      </c>
+      <c r="T82" s="4" t="str">
+        <f>IF(K82="","",ROUND(K82+M82+O82+Q82,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="83">
+      <c r="M83" s="4" t="str">
+        <f>IF(K83="","",ROUND(K83*L83/100,2))</f>
+        <v/>
+      </c>
       <c r="N83" s="2">
         <f>L83</f>
       </c>
+      <c r="O83" s="4" t="str">
+        <f>IF(K83="","",ROUND(K83*N83/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q83" s="4" t="str">
+        <f>IF(K83="","",ROUND(K83*P83/100,2))</f>
+        <v/>
+      </c>
+      <c r="T83" s="4" t="str">
+        <f>IF(K83="","",ROUND(K83+M83+O83+Q83,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="84">
+      <c r="M84" s="4" t="str">
+        <f>IF(K84="","",ROUND(K84*L84/100,2))</f>
+        <v/>
+      </c>
       <c r="N84" s="2">
         <f>L84</f>
       </c>
+      <c r="O84" s="4" t="str">
+        <f>IF(K84="","",ROUND(K84*N84/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q84" s="4" t="str">
+        <f>IF(K84="","",ROUND(K84*P84/100,2))</f>
+        <v/>
+      </c>
+      <c r="T84" s="4" t="str">
+        <f>IF(K84="","",ROUND(K84+M84+O84+Q84,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="85">
+      <c r="M85" s="4" t="str">
+        <f>IF(K85="","",ROUND(K85*L85/100,2))</f>
+        <v/>
+      </c>
       <c r="N85" s="2">
         <f>L85</f>
       </c>
+      <c r="O85" s="4" t="str">
+        <f>IF(K85="","",ROUND(K85*N85/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q85" s="4" t="str">
+        <f>IF(K85="","",ROUND(K85*P85/100,2))</f>
+        <v/>
+      </c>
+      <c r="T85" s="4" t="str">
+        <f>IF(K85="","",ROUND(K85+M85+O85+Q85,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="86">
+      <c r="M86" s="4" t="str">
+        <f>IF(K86="","",ROUND(K86*L86/100,2))</f>
+        <v/>
+      </c>
       <c r="N86" s="2">
         <f>L86</f>
       </c>
+      <c r="O86" s="4" t="str">
+        <f>IF(K86="","",ROUND(K86*N86/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q86" s="4" t="str">
+        <f>IF(K86="","",ROUND(K86*P86/100,2))</f>
+        <v/>
+      </c>
+      <c r="T86" s="4" t="str">
+        <f>IF(K86="","",ROUND(K86+M86+O86+Q86,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="87">
+      <c r="M87" s="4" t="str">
+        <f>IF(K87="","",ROUND(K87*L87/100,2))</f>
+        <v/>
+      </c>
       <c r="N87" s="2">
         <f>L87</f>
       </c>
+      <c r="O87" s="4" t="str">
+        <f>IF(K87="","",ROUND(K87*N87/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q87" s="4" t="str">
+        <f>IF(K87="","",ROUND(K87*P87/100,2))</f>
+        <v/>
+      </c>
+      <c r="T87" s="4" t="str">
+        <f>IF(K87="","",ROUND(K87+M87+O87+Q87,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="88">
+      <c r="M88" s="4" t="str">
+        <f>IF(K88="","",ROUND(K88*L88/100,2))</f>
+        <v/>
+      </c>
       <c r="N88" s="2">
         <f>L88</f>
       </c>
+      <c r="O88" s="4" t="str">
+        <f>IF(K88="","",ROUND(K88*N88/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q88" s="4" t="str">
+        <f>IF(K88="","",ROUND(K88*P88/100,2))</f>
+        <v/>
+      </c>
+      <c r="T88" s="4" t="str">
+        <f>IF(K88="","",ROUND(K88+M88+O88+Q88,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="89">
+      <c r="M89" s="4" t="str">
+        <f>IF(K89="","",ROUND(K89*L89/100,2))</f>
+        <v/>
+      </c>
       <c r="N89" s="2">
         <f>L89</f>
       </c>
+      <c r="O89" s="4" t="str">
+        <f>IF(K89="","",ROUND(K89*N89/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q89" s="4" t="str">
+        <f>IF(K89="","",ROUND(K89*P89/100,2))</f>
+        <v/>
+      </c>
+      <c r="T89" s="4" t="str">
+        <f>IF(K89="","",ROUND(K89+M89+O89+Q89,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="90">
+      <c r="M90" s="4" t="str">
+        <f>IF(K90="","",ROUND(K90*L90/100,2))</f>
+        <v/>
+      </c>
       <c r="N90" s="2">
         <f>L90</f>
       </c>
+      <c r="O90" s="4" t="str">
+        <f>IF(K90="","",ROUND(K90*N90/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q90" s="4" t="str">
+        <f>IF(K90="","",ROUND(K90*P90/100,2))</f>
+        <v/>
+      </c>
+      <c r="T90" s="4" t="str">
+        <f>IF(K90="","",ROUND(K90+M90+O90+Q90,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="91">
+      <c r="M91" s="4" t="str">
+        <f>IF(K91="","",ROUND(K91*L91/100,2))</f>
+        <v/>
+      </c>
       <c r="N91" s="2">
         <f>L91</f>
       </c>
+      <c r="O91" s="4" t="str">
+        <f>IF(K91="","",ROUND(K91*N91/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q91" s="4" t="str">
+        <f>IF(K91="","",ROUND(K91*P91/100,2))</f>
+        <v/>
+      </c>
+      <c r="T91" s="4" t="str">
+        <f>IF(K91="","",ROUND(K91+M91+O91+Q91,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="92">
+      <c r="M92" s="4" t="str">
+        <f>IF(K92="","",ROUND(K92*L92/100,2))</f>
+        <v/>
+      </c>
       <c r="N92" s="2">
         <f>L92</f>
       </c>
+      <c r="O92" s="4" t="str">
+        <f>IF(K92="","",ROUND(K92*N92/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q92" s="4" t="str">
+        <f>IF(K92="","",ROUND(K92*P92/100,2))</f>
+        <v/>
+      </c>
+      <c r="T92" s="4" t="str">
+        <f>IF(K92="","",ROUND(K92+M92+O92+Q92,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="93">
+      <c r="M93" s="4" t="str">
+        <f>IF(K93="","",ROUND(K93*L93/100,2))</f>
+        <v/>
+      </c>
       <c r="N93" s="2">
         <f>L93</f>
       </c>
+      <c r="O93" s="4" t="str">
+        <f>IF(K93="","",ROUND(K93*N93/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q93" s="4" t="str">
+        <f>IF(K93="","",ROUND(K93*P93/100,2))</f>
+        <v/>
+      </c>
+      <c r="T93" s="4" t="str">
+        <f>IF(K93="","",ROUND(K93+M93+O93+Q93,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="94">
+      <c r="M94" s="4" t="str">
+        <f>IF(K94="","",ROUND(K94*L94/100,2))</f>
+        <v/>
+      </c>
       <c r="N94" s="2">
         <f>L94</f>
       </c>
+      <c r="O94" s="4" t="str">
+        <f>IF(K94="","",ROUND(K94*N94/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q94" s="4" t="str">
+        <f>IF(K94="","",ROUND(K94*P94/100,2))</f>
+        <v/>
+      </c>
+      <c r="T94" s="4" t="str">
+        <f>IF(K94="","",ROUND(K94+M94+O94+Q94,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="95">
+      <c r="M95" s="4" t="str">
+        <f>IF(K95="","",ROUND(K95*L95/100,2))</f>
+        <v/>
+      </c>
       <c r="N95" s="2">
         <f>L95</f>
       </c>
+      <c r="O95" s="4" t="str">
+        <f>IF(K95="","",ROUND(K95*N95/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q95" s="4" t="str">
+        <f>IF(K95="","",ROUND(K95*P95/100,2))</f>
+        <v/>
+      </c>
+      <c r="T95" s="4" t="str">
+        <f>IF(K95="","",ROUND(K95+M95+O95+Q95,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="96">
+      <c r="M96" s="4" t="str">
+        <f>IF(K96="","",ROUND(K96*L96/100,2))</f>
+        <v/>
+      </c>
       <c r="N96" s="2">
         <f>L96</f>
       </c>
+      <c r="O96" s="4" t="str">
+        <f>IF(K96="","",ROUND(K96*N96/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q96" s="4" t="str">
+        <f>IF(K96="","",ROUND(K96*P96/100,2))</f>
+        <v/>
+      </c>
+      <c r="T96" s="4" t="str">
+        <f>IF(K96="","",ROUND(K96+M96+O96+Q96,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="97">
+      <c r="M97" s="4" t="str">
+        <f>IF(K97="","",ROUND(K97*L97/100,2))</f>
+        <v/>
+      </c>
       <c r="N97" s="2">
         <f>L97</f>
       </c>
+      <c r="O97" s="4" t="str">
+        <f>IF(K97="","",ROUND(K97*N97/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q97" s="4" t="str">
+        <f>IF(K97="","",ROUND(K97*P97/100,2))</f>
+        <v/>
+      </c>
+      <c r="T97" s="4" t="str">
+        <f>IF(K97="","",ROUND(K97+M97+O97+Q97,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="98">
+      <c r="M98" s="4" t="str">
+        <f>IF(K98="","",ROUND(K98*L98/100,2))</f>
+        <v/>
+      </c>
       <c r="N98" s="2">
         <f>L98</f>
       </c>
+      <c r="O98" s="4" t="str">
+        <f>IF(K98="","",ROUND(K98*N98/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q98" s="4" t="str">
+        <f>IF(K98="","",ROUND(K98*P98/100,2))</f>
+        <v/>
+      </c>
+      <c r="T98" s="4" t="str">
+        <f>IF(K98="","",ROUND(K98+M98+O98+Q98,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="99">
+      <c r="M99" s="4" t="str">
+        <f>IF(K99="","",ROUND(K99*L99/100,2))</f>
+        <v/>
+      </c>
       <c r="N99" s="2">
         <f>L99</f>
       </c>
+      <c r="O99" s="4" t="str">
+        <f>IF(K99="","",ROUND(K99*N99/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q99" s="4" t="str">
+        <f>IF(K99="","",ROUND(K99*P99/100,2))</f>
+        <v/>
+      </c>
+      <c r="T99" s="4" t="str">
+        <f>IF(K99="","",ROUND(K99+M99+O99+Q99,2))</f>
+        <v/>
+      </c>
     </row>
     <row r="100">
+      <c r="M100" s="4" t="str">
+        <f>IF(K100="","",ROUND(K100*L100/100,2))</f>
+        <v/>
+      </c>
       <c r="N100" s="2">
         <f>L100</f>
+      </c>
+      <c r="O100" s="4" t="str">
+        <f>IF(K100="","",ROUND(K100*N100/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q100" s="4" t="str">
+        <f>IF(K100="","",ROUND(K100*P100/100,2))</f>
+        <v/>
+      </c>
+      <c r="T100" s="4" t="str">
+        <f>IF(K100="","",ROUND(K100+M100+O100+Q100,2))</f>
+        <v/>
       </c>
     </row>
     <row r="101">
@@ -3077,72 +4553,1877 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" customWidth="1" width="13"/>
+    <col min="2" max="2" customWidth="1" width="16"/>
+    <col min="3" max="3" customWidth="1" width="6"/>
+    <col min="4" max="4" customWidth="1" width="13"/>
+    <col min="5" max="5" customWidth="1" width="16"/>
+    <col min="6" max="6" customWidth="1" width="20"/>
+    <col min="7" max="7" customWidth="1" width="17"/>
+    <col min="8" max="8" customWidth="1" width="18"/>
+    <col min="9" max="9" customWidth="1" width="18"/>
+    <col min="10" max="10" customWidth="1" width="10"/>
+    <col min="11" max="11" customWidth="1" width="14"/>
+    <col min="12" max="12" customWidth="1" width="8"/>
+    <col min="13" max="13" customWidth="1" width="10"/>
+    <col min="14" max="14" customWidth="1" width="8"/>
+    <col min="15" max="15" customWidth="1" width="10"/>
+    <col min="16" max="16" customWidth="1" width="8"/>
+    <col min="17" max="17" customWidth="1" width="10"/>
+    <col min="18" max="18" customWidth="1" width="7"/>
+    <col min="19" max="19" customWidth="1" width="7"/>
+    <col min="20" max="20" customWidth="1" width="8"/>
+    <col min="21" max="21" customWidth="1" width="14"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="str">
+    <row r="1" ht="27.95" customHeight="1">
+      <c r="A1" s="5" t="str">
         <v>Note Date  *</v>
       </c>
-      <c r="B1" s="2" t="str">
+      <c r="B1" s="5" t="str">
         <v>Note No.  *</v>
       </c>
-      <c r="C1" s="2" t="str">
+      <c r="C1" s="5" t="str">
         <v>C/D  *</v>
       </c>
-      <c r="D1" s="2" t="str">
+      <c r="D1" s="6" t="str">
         <v>Orig Inv Date</v>
       </c>
-      <c r="E1" s="2" t="str">
+      <c r="E1" s="6" t="str">
         <v>Orig Inv No.</v>
       </c>
-      <c r="F1" s="2" t="str">
+      <c r="F1" s="6" t="str">
         <v>Billing Name</v>
       </c>
-      <c r="G1" s="2" t="str">
+      <c r="G1" s="6" t="str">
         <v>Billing GSTIN</v>
       </c>
-      <c r="H1" s="2" t="str">
+      <c r="H1" s="5" t="str">
         <v>Place of Supply  *</v>
       </c>
-      <c r="I1" s="2" t="str">
+      <c r="I1" s="6" t="str">
         <v>Description</v>
       </c>
-      <c r="J1" s="2" t="str">
+      <c r="J1" s="6" t="str">
         <v>HSN</v>
       </c>
-      <c r="K1" s="2" t="str">
+      <c r="K1" s="5" t="str">
         <v>Taxable Value  *</v>
       </c>
-      <c r="L1" s="2" t="str">
+      <c r="L1" s="6" t="str">
         <v>CGST %</v>
       </c>
-      <c r="M1" s="2" t="str">
+      <c r="M1" s="3" t="str">
         <v>CGST Amt</v>
       </c>
-      <c r="N1" s="2" t="str">
+      <c r="N1" s="6" t="str">
         <v>SGST %</v>
       </c>
-      <c r="O1" s="2" t="str">
+      <c r="O1" s="3" t="str">
         <v>SGST Amt</v>
       </c>
-      <c r="P1" s="2" t="str">
+      <c r="P1" s="6" t="str">
         <v>IGST %</v>
       </c>
-      <c r="Q1" s="2" t="str">
+      <c r="Q1" s="3" t="str">
         <v>IGST Amt</v>
       </c>
-      <c r="R1" s="2" t="str">
+      <c r="R1" s="6" t="str">
         <v>Rev Chg</v>
       </c>
-      <c r="S1" s="2" t="str">
+      <c r="S1" s="6" t="str">
         <v>Pre GST</v>
       </c>
-      <c r="T1" s="2" t="str">
+      <c r="T1" s="6" t="str">
         <v>Rate %</v>
       </c>
-      <c r="U1" s="2" t="str">
+      <c r="U1" s="5" t="str">
         <v>Total Value  *</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="M2" s="4" t="str">
+        <f>IF(K2="","",ROUND(K2*L2/100,2))</f>
+        <v/>
+      </c>
+      <c r="O2" s="4" t="str">
+        <f>IF(K2="","",ROUND(K2*N2/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q2" s="4" t="str">
+        <f>IF(K2="","",ROUND(K2*P2/100,2))</f>
+        <v/>
+      </c>
+      <c r="U2" s="4" t="str">
+        <f>IF(K2="","",ROUND(K2+M2+O2+Q2,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="M3" s="4" t="str">
+        <f>IF(K3="","",ROUND(K3*L3/100,2))</f>
+        <v/>
+      </c>
+      <c r="O3" s="4" t="str">
+        <f>IF(K3="","",ROUND(K3*N3/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q3" s="4" t="str">
+        <f>IF(K3="","",ROUND(K3*P3/100,2))</f>
+        <v/>
+      </c>
+      <c r="U3" s="4" t="str">
+        <f>IF(K3="","",ROUND(K3+M3+O3+Q3,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="M4" s="4" t="str">
+        <f>IF(K4="","",ROUND(K4*L4/100,2))</f>
+        <v/>
+      </c>
+      <c r="O4" s="4" t="str">
+        <f>IF(K4="","",ROUND(K4*N4/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q4" s="4" t="str">
+        <f>IF(K4="","",ROUND(K4*P4/100,2))</f>
+        <v/>
+      </c>
+      <c r="U4" s="4" t="str">
+        <f>IF(K4="","",ROUND(K4+M4+O4+Q4,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="M5" s="4" t="str">
+        <f>IF(K5="","",ROUND(K5*L5/100,2))</f>
+        <v/>
+      </c>
+      <c r="O5" s="4" t="str">
+        <f>IF(K5="","",ROUND(K5*N5/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q5" s="4" t="str">
+        <f>IF(K5="","",ROUND(K5*P5/100,2))</f>
+        <v/>
+      </c>
+      <c r="U5" s="4" t="str">
+        <f>IF(K5="","",ROUND(K5+M5+O5+Q5,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="M6" s="4" t="str">
+        <f>IF(K6="","",ROUND(K6*L6/100,2))</f>
+        <v/>
+      </c>
+      <c r="O6" s="4" t="str">
+        <f>IF(K6="","",ROUND(K6*N6/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q6" s="4" t="str">
+        <f>IF(K6="","",ROUND(K6*P6/100,2))</f>
+        <v/>
+      </c>
+      <c r="U6" s="4" t="str">
+        <f>IF(K6="","",ROUND(K6+M6+O6+Q6,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="M7" s="4" t="str">
+        <f>IF(K7="","",ROUND(K7*L7/100,2))</f>
+        <v/>
+      </c>
+      <c r="O7" s="4" t="str">
+        <f>IF(K7="","",ROUND(K7*N7/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q7" s="4" t="str">
+        <f>IF(K7="","",ROUND(K7*P7/100,2))</f>
+        <v/>
+      </c>
+      <c r="U7" s="4" t="str">
+        <f>IF(K7="","",ROUND(K7+M7+O7+Q7,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="M8" s="4" t="str">
+        <f>IF(K8="","",ROUND(K8*L8/100,2))</f>
+        <v/>
+      </c>
+      <c r="O8" s="4" t="str">
+        <f>IF(K8="","",ROUND(K8*N8/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q8" s="4" t="str">
+        <f>IF(K8="","",ROUND(K8*P8/100,2))</f>
+        <v/>
+      </c>
+      <c r="U8" s="4" t="str">
+        <f>IF(K8="","",ROUND(K8+M8+O8+Q8,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="M9" s="4" t="str">
+        <f>IF(K9="","",ROUND(K9*L9/100,2))</f>
+        <v/>
+      </c>
+      <c r="O9" s="4" t="str">
+        <f>IF(K9="","",ROUND(K9*N9/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q9" s="4" t="str">
+        <f>IF(K9="","",ROUND(K9*P9/100,2))</f>
+        <v/>
+      </c>
+      <c r="U9" s="4" t="str">
+        <f>IF(K9="","",ROUND(K9+M9+O9+Q9,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="M10" s="4" t="str">
+        <f>IF(K10="","",ROUND(K10*L10/100,2))</f>
+        <v/>
+      </c>
+      <c r="O10" s="4" t="str">
+        <f>IF(K10="","",ROUND(K10*N10/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q10" s="4" t="str">
+        <f>IF(K10="","",ROUND(K10*P10/100,2))</f>
+        <v/>
+      </c>
+      <c r="U10" s="4" t="str">
+        <f>IF(K10="","",ROUND(K10+M10+O10+Q10,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="M11" s="4" t="str">
+        <f>IF(K11="","",ROUND(K11*L11/100,2))</f>
+        <v/>
+      </c>
+      <c r="O11" s="4" t="str">
+        <f>IF(K11="","",ROUND(K11*N11/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q11" s="4" t="str">
+        <f>IF(K11="","",ROUND(K11*P11/100,2))</f>
+        <v/>
+      </c>
+      <c r="U11" s="4" t="str">
+        <f>IF(K11="","",ROUND(K11+M11+O11+Q11,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="M12" s="4" t="str">
+        <f>IF(K12="","",ROUND(K12*L12/100,2))</f>
+        <v/>
+      </c>
+      <c r="O12" s="4" t="str">
+        <f>IF(K12="","",ROUND(K12*N12/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q12" s="4" t="str">
+        <f>IF(K12="","",ROUND(K12*P12/100,2))</f>
+        <v/>
+      </c>
+      <c r="U12" s="4" t="str">
+        <f>IF(K12="","",ROUND(K12+M12+O12+Q12,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="M13" s="4" t="str">
+        <f>IF(K13="","",ROUND(K13*L13/100,2))</f>
+        <v/>
+      </c>
+      <c r="O13" s="4" t="str">
+        <f>IF(K13="","",ROUND(K13*N13/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q13" s="4" t="str">
+        <f>IF(K13="","",ROUND(K13*P13/100,2))</f>
+        <v/>
+      </c>
+      <c r="U13" s="4" t="str">
+        <f>IF(K13="","",ROUND(K13+M13+O13+Q13,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="M14" s="4" t="str">
+        <f>IF(K14="","",ROUND(K14*L14/100,2))</f>
+        <v/>
+      </c>
+      <c r="O14" s="4" t="str">
+        <f>IF(K14="","",ROUND(K14*N14/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q14" s="4" t="str">
+        <f>IF(K14="","",ROUND(K14*P14/100,2))</f>
+        <v/>
+      </c>
+      <c r="U14" s="4" t="str">
+        <f>IF(K14="","",ROUND(K14+M14+O14+Q14,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="M15" s="4" t="str">
+        <f>IF(K15="","",ROUND(K15*L15/100,2))</f>
+        <v/>
+      </c>
+      <c r="O15" s="4" t="str">
+        <f>IF(K15="","",ROUND(K15*N15/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q15" s="4" t="str">
+        <f>IF(K15="","",ROUND(K15*P15/100,2))</f>
+        <v/>
+      </c>
+      <c r="U15" s="4" t="str">
+        <f>IF(K15="","",ROUND(K15+M15+O15+Q15,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="M16" s="4" t="str">
+        <f>IF(K16="","",ROUND(K16*L16/100,2))</f>
+        <v/>
+      </c>
+      <c r="O16" s="4" t="str">
+        <f>IF(K16="","",ROUND(K16*N16/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q16" s="4" t="str">
+        <f>IF(K16="","",ROUND(K16*P16/100,2))</f>
+        <v/>
+      </c>
+      <c r="U16" s="4" t="str">
+        <f>IF(K16="","",ROUND(K16+M16+O16+Q16,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="M17" s="4" t="str">
+        <f>IF(K17="","",ROUND(K17*L17/100,2))</f>
+        <v/>
+      </c>
+      <c r="O17" s="4" t="str">
+        <f>IF(K17="","",ROUND(K17*N17/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q17" s="4" t="str">
+        <f>IF(K17="","",ROUND(K17*P17/100,2))</f>
+        <v/>
+      </c>
+      <c r="U17" s="4" t="str">
+        <f>IF(K17="","",ROUND(K17+M17+O17+Q17,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="M18" s="4" t="str">
+        <f>IF(K18="","",ROUND(K18*L18/100,2))</f>
+        <v/>
+      </c>
+      <c r="O18" s="4" t="str">
+        <f>IF(K18="","",ROUND(K18*N18/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q18" s="4" t="str">
+        <f>IF(K18="","",ROUND(K18*P18/100,2))</f>
+        <v/>
+      </c>
+      <c r="U18" s="4" t="str">
+        <f>IF(K18="","",ROUND(K18+M18+O18+Q18,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="M19" s="4" t="str">
+        <f>IF(K19="","",ROUND(K19*L19/100,2))</f>
+        <v/>
+      </c>
+      <c r="O19" s="4" t="str">
+        <f>IF(K19="","",ROUND(K19*N19/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q19" s="4" t="str">
+        <f>IF(K19="","",ROUND(K19*P19/100,2))</f>
+        <v/>
+      </c>
+      <c r="U19" s="4" t="str">
+        <f>IF(K19="","",ROUND(K19+M19+O19+Q19,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="M20" s="4" t="str">
+        <f>IF(K20="","",ROUND(K20*L20/100,2))</f>
+        <v/>
+      </c>
+      <c r="O20" s="4" t="str">
+        <f>IF(K20="","",ROUND(K20*N20/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q20" s="4" t="str">
+        <f>IF(K20="","",ROUND(K20*P20/100,2))</f>
+        <v/>
+      </c>
+      <c r="U20" s="4" t="str">
+        <f>IF(K20="","",ROUND(K20+M20+O20+Q20,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="M21" s="4" t="str">
+        <f>IF(K21="","",ROUND(K21*L21/100,2))</f>
+        <v/>
+      </c>
+      <c r="O21" s="4" t="str">
+        <f>IF(K21="","",ROUND(K21*N21/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q21" s="4" t="str">
+        <f>IF(K21="","",ROUND(K21*P21/100,2))</f>
+        <v/>
+      </c>
+      <c r="U21" s="4" t="str">
+        <f>IF(K21="","",ROUND(K21+M21+O21+Q21,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="M22" s="4" t="str">
+        <f>IF(K22="","",ROUND(K22*L22/100,2))</f>
+        <v/>
+      </c>
+      <c r="O22" s="4" t="str">
+        <f>IF(K22="","",ROUND(K22*N22/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q22" s="4" t="str">
+        <f>IF(K22="","",ROUND(K22*P22/100,2))</f>
+        <v/>
+      </c>
+      <c r="U22" s="4" t="str">
+        <f>IF(K22="","",ROUND(K22+M22+O22+Q22,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="M23" s="4" t="str">
+        <f>IF(K23="","",ROUND(K23*L23/100,2))</f>
+        <v/>
+      </c>
+      <c r="O23" s="4" t="str">
+        <f>IF(K23="","",ROUND(K23*N23/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q23" s="4" t="str">
+        <f>IF(K23="","",ROUND(K23*P23/100,2))</f>
+        <v/>
+      </c>
+      <c r="U23" s="4" t="str">
+        <f>IF(K23="","",ROUND(K23+M23+O23+Q23,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="M24" s="4" t="str">
+        <f>IF(K24="","",ROUND(K24*L24/100,2))</f>
+        <v/>
+      </c>
+      <c r="O24" s="4" t="str">
+        <f>IF(K24="","",ROUND(K24*N24/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q24" s="4" t="str">
+        <f>IF(K24="","",ROUND(K24*P24/100,2))</f>
+        <v/>
+      </c>
+      <c r="U24" s="4" t="str">
+        <f>IF(K24="","",ROUND(K24+M24+O24+Q24,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="M25" s="4" t="str">
+        <f>IF(K25="","",ROUND(K25*L25/100,2))</f>
+        <v/>
+      </c>
+      <c r="O25" s="4" t="str">
+        <f>IF(K25="","",ROUND(K25*N25/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q25" s="4" t="str">
+        <f>IF(K25="","",ROUND(K25*P25/100,2))</f>
+        <v/>
+      </c>
+      <c r="U25" s="4" t="str">
+        <f>IF(K25="","",ROUND(K25+M25+O25+Q25,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="M26" s="4" t="str">
+        <f>IF(K26="","",ROUND(K26*L26/100,2))</f>
+        <v/>
+      </c>
+      <c r="O26" s="4" t="str">
+        <f>IF(K26="","",ROUND(K26*N26/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q26" s="4" t="str">
+        <f>IF(K26="","",ROUND(K26*P26/100,2))</f>
+        <v/>
+      </c>
+      <c r="U26" s="4" t="str">
+        <f>IF(K26="","",ROUND(K26+M26+O26+Q26,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="M27" s="4" t="str">
+        <f>IF(K27="","",ROUND(K27*L27/100,2))</f>
+        <v/>
+      </c>
+      <c r="O27" s="4" t="str">
+        <f>IF(K27="","",ROUND(K27*N27/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q27" s="4" t="str">
+        <f>IF(K27="","",ROUND(K27*P27/100,2))</f>
+        <v/>
+      </c>
+      <c r="U27" s="4" t="str">
+        <f>IF(K27="","",ROUND(K27+M27+O27+Q27,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="M28" s="4" t="str">
+        <f>IF(K28="","",ROUND(K28*L28/100,2))</f>
+        <v/>
+      </c>
+      <c r="O28" s="4" t="str">
+        <f>IF(K28="","",ROUND(K28*N28/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q28" s="4" t="str">
+        <f>IF(K28="","",ROUND(K28*P28/100,2))</f>
+        <v/>
+      </c>
+      <c r="U28" s="4" t="str">
+        <f>IF(K28="","",ROUND(K28+M28+O28+Q28,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="M29" s="4" t="str">
+        <f>IF(K29="","",ROUND(K29*L29/100,2))</f>
+        <v/>
+      </c>
+      <c r="O29" s="4" t="str">
+        <f>IF(K29="","",ROUND(K29*N29/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q29" s="4" t="str">
+        <f>IF(K29="","",ROUND(K29*P29/100,2))</f>
+        <v/>
+      </c>
+      <c r="U29" s="4" t="str">
+        <f>IF(K29="","",ROUND(K29+M29+O29+Q29,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="M30" s="4" t="str">
+        <f>IF(K30="","",ROUND(K30*L30/100,2))</f>
+        <v/>
+      </c>
+      <c r="O30" s="4" t="str">
+        <f>IF(K30="","",ROUND(K30*N30/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q30" s="4" t="str">
+        <f>IF(K30="","",ROUND(K30*P30/100,2))</f>
+        <v/>
+      </c>
+      <c r="U30" s="4" t="str">
+        <f>IF(K30="","",ROUND(K30+M30+O30+Q30,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="M31" s="4" t="str">
+        <f>IF(K31="","",ROUND(K31*L31/100,2))</f>
+        <v/>
+      </c>
+      <c r="O31" s="4" t="str">
+        <f>IF(K31="","",ROUND(K31*N31/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q31" s="4" t="str">
+        <f>IF(K31="","",ROUND(K31*P31/100,2))</f>
+        <v/>
+      </c>
+      <c r="U31" s="4" t="str">
+        <f>IF(K31="","",ROUND(K31+M31+O31+Q31,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="M32" s="4" t="str">
+        <f>IF(K32="","",ROUND(K32*L32/100,2))</f>
+        <v/>
+      </c>
+      <c r="O32" s="4" t="str">
+        <f>IF(K32="","",ROUND(K32*N32/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q32" s="4" t="str">
+        <f>IF(K32="","",ROUND(K32*P32/100,2))</f>
+        <v/>
+      </c>
+      <c r="U32" s="4" t="str">
+        <f>IF(K32="","",ROUND(K32+M32+O32+Q32,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="M33" s="4" t="str">
+        <f>IF(K33="","",ROUND(K33*L33/100,2))</f>
+        <v/>
+      </c>
+      <c r="O33" s="4" t="str">
+        <f>IF(K33="","",ROUND(K33*N33/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q33" s="4" t="str">
+        <f>IF(K33="","",ROUND(K33*P33/100,2))</f>
+        <v/>
+      </c>
+      <c r="U33" s="4" t="str">
+        <f>IF(K33="","",ROUND(K33+M33+O33+Q33,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="M34" s="4" t="str">
+        <f>IF(K34="","",ROUND(K34*L34/100,2))</f>
+        <v/>
+      </c>
+      <c r="O34" s="4" t="str">
+        <f>IF(K34="","",ROUND(K34*N34/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q34" s="4" t="str">
+        <f>IF(K34="","",ROUND(K34*P34/100,2))</f>
+        <v/>
+      </c>
+      <c r="U34" s="4" t="str">
+        <f>IF(K34="","",ROUND(K34+M34+O34+Q34,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="M35" s="4" t="str">
+        <f>IF(K35="","",ROUND(K35*L35/100,2))</f>
+        <v/>
+      </c>
+      <c r="O35" s="4" t="str">
+        <f>IF(K35="","",ROUND(K35*N35/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q35" s="4" t="str">
+        <f>IF(K35="","",ROUND(K35*P35/100,2))</f>
+        <v/>
+      </c>
+      <c r="U35" s="4" t="str">
+        <f>IF(K35="","",ROUND(K35+M35+O35+Q35,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="M36" s="4" t="str">
+        <f>IF(K36="","",ROUND(K36*L36/100,2))</f>
+        <v/>
+      </c>
+      <c r="O36" s="4" t="str">
+        <f>IF(K36="","",ROUND(K36*N36/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q36" s="4" t="str">
+        <f>IF(K36="","",ROUND(K36*P36/100,2))</f>
+        <v/>
+      </c>
+      <c r="U36" s="4" t="str">
+        <f>IF(K36="","",ROUND(K36+M36+O36+Q36,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="M37" s="4" t="str">
+        <f>IF(K37="","",ROUND(K37*L37/100,2))</f>
+        <v/>
+      </c>
+      <c r="O37" s="4" t="str">
+        <f>IF(K37="","",ROUND(K37*N37/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q37" s="4" t="str">
+        <f>IF(K37="","",ROUND(K37*P37/100,2))</f>
+        <v/>
+      </c>
+      <c r="U37" s="4" t="str">
+        <f>IF(K37="","",ROUND(K37+M37+O37+Q37,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="M38" s="4" t="str">
+        <f>IF(K38="","",ROUND(K38*L38/100,2))</f>
+        <v/>
+      </c>
+      <c r="O38" s="4" t="str">
+        <f>IF(K38="","",ROUND(K38*N38/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q38" s="4" t="str">
+        <f>IF(K38="","",ROUND(K38*P38/100,2))</f>
+        <v/>
+      </c>
+      <c r="U38" s="4" t="str">
+        <f>IF(K38="","",ROUND(K38+M38+O38+Q38,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="M39" s="4" t="str">
+        <f>IF(K39="","",ROUND(K39*L39/100,2))</f>
+        <v/>
+      </c>
+      <c r="O39" s="4" t="str">
+        <f>IF(K39="","",ROUND(K39*N39/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q39" s="4" t="str">
+        <f>IF(K39="","",ROUND(K39*P39/100,2))</f>
+        <v/>
+      </c>
+      <c r="U39" s="4" t="str">
+        <f>IF(K39="","",ROUND(K39+M39+O39+Q39,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="M40" s="4" t="str">
+        <f>IF(K40="","",ROUND(K40*L40/100,2))</f>
+        <v/>
+      </c>
+      <c r="O40" s="4" t="str">
+        <f>IF(K40="","",ROUND(K40*N40/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q40" s="4" t="str">
+        <f>IF(K40="","",ROUND(K40*P40/100,2))</f>
+        <v/>
+      </c>
+      <c r="U40" s="4" t="str">
+        <f>IF(K40="","",ROUND(K40+M40+O40+Q40,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="M41" s="4" t="str">
+        <f>IF(K41="","",ROUND(K41*L41/100,2))</f>
+        <v/>
+      </c>
+      <c r="O41" s="4" t="str">
+        <f>IF(K41="","",ROUND(K41*N41/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q41" s="4" t="str">
+        <f>IF(K41="","",ROUND(K41*P41/100,2))</f>
+        <v/>
+      </c>
+      <c r="U41" s="4" t="str">
+        <f>IF(K41="","",ROUND(K41+M41+O41+Q41,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="M42" s="4" t="str">
+        <f>IF(K42="","",ROUND(K42*L42/100,2))</f>
+        <v/>
+      </c>
+      <c r="O42" s="4" t="str">
+        <f>IF(K42="","",ROUND(K42*N42/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q42" s="4" t="str">
+        <f>IF(K42="","",ROUND(K42*P42/100,2))</f>
+        <v/>
+      </c>
+      <c r="U42" s="4" t="str">
+        <f>IF(K42="","",ROUND(K42+M42+O42+Q42,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="M43" s="4" t="str">
+        <f>IF(K43="","",ROUND(K43*L43/100,2))</f>
+        <v/>
+      </c>
+      <c r="O43" s="4" t="str">
+        <f>IF(K43="","",ROUND(K43*N43/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q43" s="4" t="str">
+        <f>IF(K43="","",ROUND(K43*P43/100,2))</f>
+        <v/>
+      </c>
+      <c r="U43" s="4" t="str">
+        <f>IF(K43="","",ROUND(K43+M43+O43+Q43,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="M44" s="4" t="str">
+        <f>IF(K44="","",ROUND(K44*L44/100,2))</f>
+        <v/>
+      </c>
+      <c r="O44" s="4" t="str">
+        <f>IF(K44="","",ROUND(K44*N44/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q44" s="4" t="str">
+        <f>IF(K44="","",ROUND(K44*P44/100,2))</f>
+        <v/>
+      </c>
+      <c r="U44" s="4" t="str">
+        <f>IF(K44="","",ROUND(K44+M44+O44+Q44,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="M45" s="4" t="str">
+        <f>IF(K45="","",ROUND(K45*L45/100,2))</f>
+        <v/>
+      </c>
+      <c r="O45" s="4" t="str">
+        <f>IF(K45="","",ROUND(K45*N45/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q45" s="4" t="str">
+        <f>IF(K45="","",ROUND(K45*P45/100,2))</f>
+        <v/>
+      </c>
+      <c r="U45" s="4" t="str">
+        <f>IF(K45="","",ROUND(K45+M45+O45+Q45,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="M46" s="4" t="str">
+        <f>IF(K46="","",ROUND(K46*L46/100,2))</f>
+        <v/>
+      </c>
+      <c r="O46" s="4" t="str">
+        <f>IF(K46="","",ROUND(K46*N46/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q46" s="4" t="str">
+        <f>IF(K46="","",ROUND(K46*P46/100,2))</f>
+        <v/>
+      </c>
+      <c r="U46" s="4" t="str">
+        <f>IF(K46="","",ROUND(K46+M46+O46+Q46,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="M47" s="4" t="str">
+        <f>IF(K47="","",ROUND(K47*L47/100,2))</f>
+        <v/>
+      </c>
+      <c r="O47" s="4" t="str">
+        <f>IF(K47="","",ROUND(K47*N47/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q47" s="4" t="str">
+        <f>IF(K47="","",ROUND(K47*P47/100,2))</f>
+        <v/>
+      </c>
+      <c r="U47" s="4" t="str">
+        <f>IF(K47="","",ROUND(K47+M47+O47+Q47,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="M48" s="4" t="str">
+        <f>IF(K48="","",ROUND(K48*L48/100,2))</f>
+        <v/>
+      </c>
+      <c r="O48" s="4" t="str">
+        <f>IF(K48="","",ROUND(K48*N48/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q48" s="4" t="str">
+        <f>IF(K48="","",ROUND(K48*P48/100,2))</f>
+        <v/>
+      </c>
+      <c r="U48" s="4" t="str">
+        <f>IF(K48="","",ROUND(K48+M48+O48+Q48,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="M49" s="4" t="str">
+        <f>IF(K49="","",ROUND(K49*L49/100,2))</f>
+        <v/>
+      </c>
+      <c r="O49" s="4" t="str">
+        <f>IF(K49="","",ROUND(K49*N49/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q49" s="4" t="str">
+        <f>IF(K49="","",ROUND(K49*P49/100,2))</f>
+        <v/>
+      </c>
+      <c r="U49" s="4" t="str">
+        <f>IF(K49="","",ROUND(K49+M49+O49+Q49,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="M50" s="4" t="str">
+        <f>IF(K50="","",ROUND(K50*L50/100,2))</f>
+        <v/>
+      </c>
+      <c r="O50" s="4" t="str">
+        <f>IF(K50="","",ROUND(K50*N50/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q50" s="4" t="str">
+        <f>IF(K50="","",ROUND(K50*P50/100,2))</f>
+        <v/>
+      </c>
+      <c r="U50" s="4" t="str">
+        <f>IF(K50="","",ROUND(K50+M50+O50+Q50,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="M51" s="4" t="str">
+        <f>IF(K51="","",ROUND(K51*L51/100,2))</f>
+        <v/>
+      </c>
+      <c r="O51" s="4" t="str">
+        <f>IF(K51="","",ROUND(K51*N51/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q51" s="4" t="str">
+        <f>IF(K51="","",ROUND(K51*P51/100,2))</f>
+        <v/>
+      </c>
+      <c r="U51" s="4" t="str">
+        <f>IF(K51="","",ROUND(K51+M51+O51+Q51,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52">
+      <c r="M52" s="4" t="str">
+        <f>IF(K52="","",ROUND(K52*L52/100,2))</f>
+        <v/>
+      </c>
+      <c r="O52" s="4" t="str">
+        <f>IF(K52="","",ROUND(K52*N52/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q52" s="4" t="str">
+        <f>IF(K52="","",ROUND(K52*P52/100,2))</f>
+        <v/>
+      </c>
+      <c r="U52" s="4" t="str">
+        <f>IF(K52="","",ROUND(K52+M52+O52+Q52,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53">
+      <c r="M53" s="4" t="str">
+        <f>IF(K53="","",ROUND(K53*L53/100,2))</f>
+        <v/>
+      </c>
+      <c r="O53" s="4" t="str">
+        <f>IF(K53="","",ROUND(K53*N53/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q53" s="4" t="str">
+        <f>IF(K53="","",ROUND(K53*P53/100,2))</f>
+        <v/>
+      </c>
+      <c r="U53" s="4" t="str">
+        <f>IF(K53="","",ROUND(K53+M53+O53+Q53,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54">
+      <c r="M54" s="4" t="str">
+        <f>IF(K54="","",ROUND(K54*L54/100,2))</f>
+        <v/>
+      </c>
+      <c r="O54" s="4" t="str">
+        <f>IF(K54="","",ROUND(K54*N54/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q54" s="4" t="str">
+        <f>IF(K54="","",ROUND(K54*P54/100,2))</f>
+        <v/>
+      </c>
+      <c r="U54" s="4" t="str">
+        <f>IF(K54="","",ROUND(K54+M54+O54+Q54,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55">
+      <c r="M55" s="4" t="str">
+        <f>IF(K55="","",ROUND(K55*L55/100,2))</f>
+        <v/>
+      </c>
+      <c r="O55" s="4" t="str">
+        <f>IF(K55="","",ROUND(K55*N55/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q55" s="4" t="str">
+        <f>IF(K55="","",ROUND(K55*P55/100,2))</f>
+        <v/>
+      </c>
+      <c r="U55" s="4" t="str">
+        <f>IF(K55="","",ROUND(K55+M55+O55+Q55,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56">
+      <c r="M56" s="4" t="str">
+        <f>IF(K56="","",ROUND(K56*L56/100,2))</f>
+        <v/>
+      </c>
+      <c r="O56" s="4" t="str">
+        <f>IF(K56="","",ROUND(K56*N56/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q56" s="4" t="str">
+        <f>IF(K56="","",ROUND(K56*P56/100,2))</f>
+        <v/>
+      </c>
+      <c r="U56" s="4" t="str">
+        <f>IF(K56="","",ROUND(K56+M56+O56+Q56,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57">
+      <c r="M57" s="4" t="str">
+        <f>IF(K57="","",ROUND(K57*L57/100,2))</f>
+        <v/>
+      </c>
+      <c r="O57" s="4" t="str">
+        <f>IF(K57="","",ROUND(K57*N57/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q57" s="4" t="str">
+        <f>IF(K57="","",ROUND(K57*P57/100,2))</f>
+        <v/>
+      </c>
+      <c r="U57" s="4" t="str">
+        <f>IF(K57="","",ROUND(K57+M57+O57+Q57,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58">
+      <c r="M58" s="4" t="str">
+        <f>IF(K58="","",ROUND(K58*L58/100,2))</f>
+        <v/>
+      </c>
+      <c r="O58" s="4" t="str">
+        <f>IF(K58="","",ROUND(K58*N58/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q58" s="4" t="str">
+        <f>IF(K58="","",ROUND(K58*P58/100,2))</f>
+        <v/>
+      </c>
+      <c r="U58" s="4" t="str">
+        <f>IF(K58="","",ROUND(K58+M58+O58+Q58,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="M59" s="4" t="str">
+        <f>IF(K59="","",ROUND(K59*L59/100,2))</f>
+        <v/>
+      </c>
+      <c r="O59" s="4" t="str">
+        <f>IF(K59="","",ROUND(K59*N59/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q59" s="4" t="str">
+        <f>IF(K59="","",ROUND(K59*P59/100,2))</f>
+        <v/>
+      </c>
+      <c r="U59" s="4" t="str">
+        <f>IF(K59="","",ROUND(K59+M59+O59+Q59,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="M60" s="4" t="str">
+        <f>IF(K60="","",ROUND(K60*L60/100,2))</f>
+        <v/>
+      </c>
+      <c r="O60" s="4" t="str">
+        <f>IF(K60="","",ROUND(K60*N60/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q60" s="4" t="str">
+        <f>IF(K60="","",ROUND(K60*P60/100,2))</f>
+        <v/>
+      </c>
+      <c r="U60" s="4" t="str">
+        <f>IF(K60="","",ROUND(K60+M60+O60+Q60,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61">
+      <c r="M61" s="4" t="str">
+        <f>IF(K61="","",ROUND(K61*L61/100,2))</f>
+        <v/>
+      </c>
+      <c r="O61" s="4" t="str">
+        <f>IF(K61="","",ROUND(K61*N61/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q61" s="4" t="str">
+        <f>IF(K61="","",ROUND(K61*P61/100,2))</f>
+        <v/>
+      </c>
+      <c r="U61" s="4" t="str">
+        <f>IF(K61="","",ROUND(K61+M61+O61+Q61,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62">
+      <c r="M62" s="4" t="str">
+        <f>IF(K62="","",ROUND(K62*L62/100,2))</f>
+        <v/>
+      </c>
+      <c r="O62" s="4" t="str">
+        <f>IF(K62="","",ROUND(K62*N62/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q62" s="4" t="str">
+        <f>IF(K62="","",ROUND(K62*P62/100,2))</f>
+        <v/>
+      </c>
+      <c r="U62" s="4" t="str">
+        <f>IF(K62="","",ROUND(K62+M62+O62+Q62,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63">
+      <c r="M63" s="4" t="str">
+        <f>IF(K63="","",ROUND(K63*L63/100,2))</f>
+        <v/>
+      </c>
+      <c r="O63" s="4" t="str">
+        <f>IF(K63="","",ROUND(K63*N63/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q63" s="4" t="str">
+        <f>IF(K63="","",ROUND(K63*P63/100,2))</f>
+        <v/>
+      </c>
+      <c r="U63" s="4" t="str">
+        <f>IF(K63="","",ROUND(K63+M63+O63+Q63,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64">
+      <c r="M64" s="4" t="str">
+        <f>IF(K64="","",ROUND(K64*L64/100,2))</f>
+        <v/>
+      </c>
+      <c r="O64" s="4" t="str">
+        <f>IF(K64="","",ROUND(K64*N64/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q64" s="4" t="str">
+        <f>IF(K64="","",ROUND(K64*P64/100,2))</f>
+        <v/>
+      </c>
+      <c r="U64" s="4" t="str">
+        <f>IF(K64="","",ROUND(K64+M64+O64+Q64,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="M65" s="4" t="str">
+        <f>IF(K65="","",ROUND(K65*L65/100,2))</f>
+        <v/>
+      </c>
+      <c r="O65" s="4" t="str">
+        <f>IF(K65="","",ROUND(K65*N65/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q65" s="4" t="str">
+        <f>IF(K65="","",ROUND(K65*P65/100,2))</f>
+        <v/>
+      </c>
+      <c r="U65" s="4" t="str">
+        <f>IF(K65="","",ROUND(K65+M65+O65+Q65,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66">
+      <c r="M66" s="4" t="str">
+        <f>IF(K66="","",ROUND(K66*L66/100,2))</f>
+        <v/>
+      </c>
+      <c r="O66" s="4" t="str">
+        <f>IF(K66="","",ROUND(K66*N66/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q66" s="4" t="str">
+        <f>IF(K66="","",ROUND(K66*P66/100,2))</f>
+        <v/>
+      </c>
+      <c r="U66" s="4" t="str">
+        <f>IF(K66="","",ROUND(K66+M66+O66+Q66,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="M67" s="4" t="str">
+        <f>IF(K67="","",ROUND(K67*L67/100,2))</f>
+        <v/>
+      </c>
+      <c r="O67" s="4" t="str">
+        <f>IF(K67="","",ROUND(K67*N67/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q67" s="4" t="str">
+        <f>IF(K67="","",ROUND(K67*P67/100,2))</f>
+        <v/>
+      </c>
+      <c r="U67" s="4" t="str">
+        <f>IF(K67="","",ROUND(K67+M67+O67+Q67,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68">
+      <c r="M68" s="4" t="str">
+        <f>IF(K68="","",ROUND(K68*L68/100,2))</f>
+        <v/>
+      </c>
+      <c r="O68" s="4" t="str">
+        <f>IF(K68="","",ROUND(K68*N68/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q68" s="4" t="str">
+        <f>IF(K68="","",ROUND(K68*P68/100,2))</f>
+        <v/>
+      </c>
+      <c r="U68" s="4" t="str">
+        <f>IF(K68="","",ROUND(K68+M68+O68+Q68,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69">
+      <c r="M69" s="4" t="str">
+        <f>IF(K69="","",ROUND(K69*L69/100,2))</f>
+        <v/>
+      </c>
+      <c r="O69" s="4" t="str">
+        <f>IF(K69="","",ROUND(K69*N69/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q69" s="4" t="str">
+        <f>IF(K69="","",ROUND(K69*P69/100,2))</f>
+        <v/>
+      </c>
+      <c r="U69" s="4" t="str">
+        <f>IF(K69="","",ROUND(K69+M69+O69+Q69,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70">
+      <c r="M70" s="4" t="str">
+        <f>IF(K70="","",ROUND(K70*L70/100,2))</f>
+        <v/>
+      </c>
+      <c r="O70" s="4" t="str">
+        <f>IF(K70="","",ROUND(K70*N70/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q70" s="4" t="str">
+        <f>IF(K70="","",ROUND(K70*P70/100,2))</f>
+        <v/>
+      </c>
+      <c r="U70" s="4" t="str">
+        <f>IF(K70="","",ROUND(K70+M70+O70+Q70,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="M71" s="4" t="str">
+        <f>IF(K71="","",ROUND(K71*L71/100,2))</f>
+        <v/>
+      </c>
+      <c r="O71" s="4" t="str">
+        <f>IF(K71="","",ROUND(K71*N71/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q71" s="4" t="str">
+        <f>IF(K71="","",ROUND(K71*P71/100,2))</f>
+        <v/>
+      </c>
+      <c r="U71" s="4" t="str">
+        <f>IF(K71="","",ROUND(K71+M71+O71+Q71,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72">
+      <c r="M72" s="4" t="str">
+        <f>IF(K72="","",ROUND(K72*L72/100,2))</f>
+        <v/>
+      </c>
+      <c r="O72" s="4" t="str">
+        <f>IF(K72="","",ROUND(K72*N72/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q72" s="4" t="str">
+        <f>IF(K72="","",ROUND(K72*P72/100,2))</f>
+        <v/>
+      </c>
+      <c r="U72" s="4" t="str">
+        <f>IF(K72="","",ROUND(K72+M72+O72+Q72,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73">
+      <c r="M73" s="4" t="str">
+        <f>IF(K73="","",ROUND(K73*L73/100,2))</f>
+        <v/>
+      </c>
+      <c r="O73" s="4" t="str">
+        <f>IF(K73="","",ROUND(K73*N73/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q73" s="4" t="str">
+        <f>IF(K73="","",ROUND(K73*P73/100,2))</f>
+        <v/>
+      </c>
+      <c r="U73" s="4" t="str">
+        <f>IF(K73="","",ROUND(K73+M73+O73+Q73,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="M74" s="4" t="str">
+        <f>IF(K74="","",ROUND(K74*L74/100,2))</f>
+        <v/>
+      </c>
+      <c r="O74" s="4" t="str">
+        <f>IF(K74="","",ROUND(K74*N74/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q74" s="4" t="str">
+        <f>IF(K74="","",ROUND(K74*P74/100,2))</f>
+        <v/>
+      </c>
+      <c r="U74" s="4" t="str">
+        <f>IF(K74="","",ROUND(K74+M74+O74+Q74,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75">
+      <c r="M75" s="4" t="str">
+        <f>IF(K75="","",ROUND(K75*L75/100,2))</f>
+        <v/>
+      </c>
+      <c r="O75" s="4" t="str">
+        <f>IF(K75="","",ROUND(K75*N75/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q75" s="4" t="str">
+        <f>IF(K75="","",ROUND(K75*P75/100,2))</f>
+        <v/>
+      </c>
+      <c r="U75" s="4" t="str">
+        <f>IF(K75="","",ROUND(K75+M75+O75+Q75,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76">
+      <c r="M76" s="4" t="str">
+        <f>IF(K76="","",ROUND(K76*L76/100,2))</f>
+        <v/>
+      </c>
+      <c r="O76" s="4" t="str">
+        <f>IF(K76="","",ROUND(K76*N76/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q76" s="4" t="str">
+        <f>IF(K76="","",ROUND(K76*P76/100,2))</f>
+        <v/>
+      </c>
+      <c r="U76" s="4" t="str">
+        <f>IF(K76="","",ROUND(K76+M76+O76+Q76,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77">
+      <c r="M77" s="4" t="str">
+        <f>IF(K77="","",ROUND(K77*L77/100,2))</f>
+        <v/>
+      </c>
+      <c r="O77" s="4" t="str">
+        <f>IF(K77="","",ROUND(K77*N77/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q77" s="4" t="str">
+        <f>IF(K77="","",ROUND(K77*P77/100,2))</f>
+        <v/>
+      </c>
+      <c r="U77" s="4" t="str">
+        <f>IF(K77="","",ROUND(K77+M77+O77+Q77,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78">
+      <c r="M78" s="4" t="str">
+        <f>IF(K78="","",ROUND(K78*L78/100,2))</f>
+        <v/>
+      </c>
+      <c r="O78" s="4" t="str">
+        <f>IF(K78="","",ROUND(K78*N78/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q78" s="4" t="str">
+        <f>IF(K78="","",ROUND(K78*P78/100,2))</f>
+        <v/>
+      </c>
+      <c r="U78" s="4" t="str">
+        <f>IF(K78="","",ROUND(K78+M78+O78+Q78,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="M79" s="4" t="str">
+        <f>IF(K79="","",ROUND(K79*L79/100,2))</f>
+        <v/>
+      </c>
+      <c r="O79" s="4" t="str">
+        <f>IF(K79="","",ROUND(K79*N79/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q79" s="4" t="str">
+        <f>IF(K79="","",ROUND(K79*P79/100,2))</f>
+        <v/>
+      </c>
+      <c r="U79" s="4" t="str">
+        <f>IF(K79="","",ROUND(K79+M79+O79+Q79,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80">
+      <c r="M80" s="4" t="str">
+        <f>IF(K80="","",ROUND(K80*L80/100,2))</f>
+        <v/>
+      </c>
+      <c r="O80" s="4" t="str">
+        <f>IF(K80="","",ROUND(K80*N80/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q80" s="4" t="str">
+        <f>IF(K80="","",ROUND(K80*P80/100,2))</f>
+        <v/>
+      </c>
+      <c r="U80" s="4" t="str">
+        <f>IF(K80="","",ROUND(K80+M80+O80+Q80,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81">
+      <c r="M81" s="4" t="str">
+        <f>IF(K81="","",ROUND(K81*L81/100,2))</f>
+        <v/>
+      </c>
+      <c r="O81" s="4" t="str">
+        <f>IF(K81="","",ROUND(K81*N81/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q81" s="4" t="str">
+        <f>IF(K81="","",ROUND(K81*P81/100,2))</f>
+        <v/>
+      </c>
+      <c r="U81" s="4" t="str">
+        <f>IF(K81="","",ROUND(K81+M81+O81+Q81,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82">
+      <c r="M82" s="4" t="str">
+        <f>IF(K82="","",ROUND(K82*L82/100,2))</f>
+        <v/>
+      </c>
+      <c r="O82" s="4" t="str">
+        <f>IF(K82="","",ROUND(K82*N82/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q82" s="4" t="str">
+        <f>IF(K82="","",ROUND(K82*P82/100,2))</f>
+        <v/>
+      </c>
+      <c r="U82" s="4" t="str">
+        <f>IF(K82="","",ROUND(K82+M82+O82+Q82,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83">
+      <c r="M83" s="4" t="str">
+        <f>IF(K83="","",ROUND(K83*L83/100,2))</f>
+        <v/>
+      </c>
+      <c r="O83" s="4" t="str">
+        <f>IF(K83="","",ROUND(K83*N83/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q83" s="4" t="str">
+        <f>IF(K83="","",ROUND(K83*P83/100,2))</f>
+        <v/>
+      </c>
+      <c r="U83" s="4" t="str">
+        <f>IF(K83="","",ROUND(K83+M83+O83+Q83,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84">
+      <c r="M84" s="4" t="str">
+        <f>IF(K84="","",ROUND(K84*L84/100,2))</f>
+        <v/>
+      </c>
+      <c r="O84" s="4" t="str">
+        <f>IF(K84="","",ROUND(K84*N84/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q84" s="4" t="str">
+        <f>IF(K84="","",ROUND(K84*P84/100,2))</f>
+        <v/>
+      </c>
+      <c r="U84" s="4" t="str">
+        <f>IF(K84="","",ROUND(K84+M84+O84+Q84,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85">
+      <c r="M85" s="4" t="str">
+        <f>IF(K85="","",ROUND(K85*L85/100,2))</f>
+        <v/>
+      </c>
+      <c r="O85" s="4" t="str">
+        <f>IF(K85="","",ROUND(K85*N85/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q85" s="4" t="str">
+        <f>IF(K85="","",ROUND(K85*P85/100,2))</f>
+        <v/>
+      </c>
+      <c r="U85" s="4" t="str">
+        <f>IF(K85="","",ROUND(K85+M85+O85+Q85,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86">
+      <c r="M86" s="4" t="str">
+        <f>IF(K86="","",ROUND(K86*L86/100,2))</f>
+        <v/>
+      </c>
+      <c r="O86" s="4" t="str">
+        <f>IF(K86="","",ROUND(K86*N86/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q86" s="4" t="str">
+        <f>IF(K86="","",ROUND(K86*P86/100,2))</f>
+        <v/>
+      </c>
+      <c r="U86" s="4" t="str">
+        <f>IF(K86="","",ROUND(K86+M86+O86+Q86,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87">
+      <c r="M87" s="4" t="str">
+        <f>IF(K87="","",ROUND(K87*L87/100,2))</f>
+        <v/>
+      </c>
+      <c r="O87" s="4" t="str">
+        <f>IF(K87="","",ROUND(K87*N87/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q87" s="4" t="str">
+        <f>IF(K87="","",ROUND(K87*P87/100,2))</f>
+        <v/>
+      </c>
+      <c r="U87" s="4" t="str">
+        <f>IF(K87="","",ROUND(K87+M87+O87+Q87,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88">
+      <c r="M88" s="4" t="str">
+        <f>IF(K88="","",ROUND(K88*L88/100,2))</f>
+        <v/>
+      </c>
+      <c r="O88" s="4" t="str">
+        <f>IF(K88="","",ROUND(K88*N88/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q88" s="4" t="str">
+        <f>IF(K88="","",ROUND(K88*P88/100,2))</f>
+        <v/>
+      </c>
+      <c r="U88" s="4" t="str">
+        <f>IF(K88="","",ROUND(K88+M88+O88+Q88,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89">
+      <c r="M89" s="4" t="str">
+        <f>IF(K89="","",ROUND(K89*L89/100,2))</f>
+        <v/>
+      </c>
+      <c r="O89" s="4" t="str">
+        <f>IF(K89="","",ROUND(K89*N89/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q89" s="4" t="str">
+        <f>IF(K89="","",ROUND(K89*P89/100,2))</f>
+        <v/>
+      </c>
+      <c r="U89" s="4" t="str">
+        <f>IF(K89="","",ROUND(K89+M89+O89+Q89,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90">
+      <c r="M90" s="4" t="str">
+        <f>IF(K90="","",ROUND(K90*L90/100,2))</f>
+        <v/>
+      </c>
+      <c r="O90" s="4" t="str">
+        <f>IF(K90="","",ROUND(K90*N90/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q90" s="4" t="str">
+        <f>IF(K90="","",ROUND(K90*P90/100,2))</f>
+        <v/>
+      </c>
+      <c r="U90" s="4" t="str">
+        <f>IF(K90="","",ROUND(K90+M90+O90+Q90,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91">
+      <c r="M91" s="4" t="str">
+        <f>IF(K91="","",ROUND(K91*L91/100,2))</f>
+        <v/>
+      </c>
+      <c r="O91" s="4" t="str">
+        <f>IF(K91="","",ROUND(K91*N91/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q91" s="4" t="str">
+        <f>IF(K91="","",ROUND(K91*P91/100,2))</f>
+        <v/>
+      </c>
+      <c r="U91" s="4" t="str">
+        <f>IF(K91="","",ROUND(K91+M91+O91+Q91,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92">
+      <c r="M92" s="4" t="str">
+        <f>IF(K92="","",ROUND(K92*L92/100,2))</f>
+        <v/>
+      </c>
+      <c r="O92" s="4" t="str">
+        <f>IF(K92="","",ROUND(K92*N92/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q92" s="4" t="str">
+        <f>IF(K92="","",ROUND(K92*P92/100,2))</f>
+        <v/>
+      </c>
+      <c r="U92" s="4" t="str">
+        <f>IF(K92="","",ROUND(K92+M92+O92+Q92,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93">
+      <c r="M93" s="4" t="str">
+        <f>IF(K93="","",ROUND(K93*L93/100,2))</f>
+        <v/>
+      </c>
+      <c r="O93" s="4" t="str">
+        <f>IF(K93="","",ROUND(K93*N93/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q93" s="4" t="str">
+        <f>IF(K93="","",ROUND(K93*P93/100,2))</f>
+        <v/>
+      </c>
+      <c r="U93" s="4" t="str">
+        <f>IF(K93="","",ROUND(K93+M93+O93+Q93,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94">
+      <c r="M94" s="4" t="str">
+        <f>IF(K94="","",ROUND(K94*L94/100,2))</f>
+        <v/>
+      </c>
+      <c r="O94" s="4" t="str">
+        <f>IF(K94="","",ROUND(K94*N94/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q94" s="4" t="str">
+        <f>IF(K94="","",ROUND(K94*P94/100,2))</f>
+        <v/>
+      </c>
+      <c r="U94" s="4" t="str">
+        <f>IF(K94="","",ROUND(K94+M94+O94+Q94,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95">
+      <c r="M95" s="4" t="str">
+        <f>IF(K95="","",ROUND(K95*L95/100,2))</f>
+        <v/>
+      </c>
+      <c r="O95" s="4" t="str">
+        <f>IF(K95="","",ROUND(K95*N95/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q95" s="4" t="str">
+        <f>IF(K95="","",ROUND(K95*P95/100,2))</f>
+        <v/>
+      </c>
+      <c r="U95" s="4" t="str">
+        <f>IF(K95="","",ROUND(K95+M95+O95+Q95,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96">
+      <c r="M96" s="4" t="str">
+        <f>IF(K96="","",ROUND(K96*L96/100,2))</f>
+        <v/>
+      </c>
+      <c r="O96" s="4" t="str">
+        <f>IF(K96="","",ROUND(K96*N96/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q96" s="4" t="str">
+        <f>IF(K96="","",ROUND(K96*P96/100,2))</f>
+        <v/>
+      </c>
+      <c r="U96" s="4" t="str">
+        <f>IF(K96="","",ROUND(K96+M96+O96+Q96,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97">
+      <c r="M97" s="4" t="str">
+        <f>IF(K97="","",ROUND(K97*L97/100,2))</f>
+        <v/>
+      </c>
+      <c r="O97" s="4" t="str">
+        <f>IF(K97="","",ROUND(K97*N97/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q97" s="4" t="str">
+        <f>IF(K97="","",ROUND(K97*P97/100,2))</f>
+        <v/>
+      </c>
+      <c r="U97" s="4" t="str">
+        <f>IF(K97="","",ROUND(K97+M97+O97+Q97,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98">
+      <c r="M98" s="4" t="str">
+        <f>IF(K98="","",ROUND(K98*L98/100,2))</f>
+        <v/>
+      </c>
+      <c r="O98" s="4" t="str">
+        <f>IF(K98="","",ROUND(K98*N98/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q98" s="4" t="str">
+        <f>IF(K98="","",ROUND(K98*P98/100,2))</f>
+        <v/>
+      </c>
+      <c r="U98" s="4" t="str">
+        <f>IF(K98="","",ROUND(K98+M98+O98+Q98,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99">
+      <c r="M99" s="4" t="str">
+        <f>IF(K99="","",ROUND(K99*L99/100,2))</f>
+        <v/>
+      </c>
+      <c r="O99" s="4" t="str">
+        <f>IF(K99="","",ROUND(K99*N99/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q99" s="4" t="str">
+        <f>IF(K99="","",ROUND(K99*P99/100,2))</f>
+        <v/>
+      </c>
+      <c r="U99" s="4" t="str">
+        <f>IF(K99="","",ROUND(K99+M99+O99+Q99,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100">
+      <c r="M100" s="4" t="str">
+        <f>IF(K100="","",ROUND(K100*L100/100,2))</f>
+        <v/>
+      </c>
+      <c r="O100" s="4" t="str">
+        <f>IF(K100="","",ROUND(K100*N100/100,2))</f>
+        <v/>
+      </c>
+      <c r="Q100" s="4" t="str">
+        <f>IF(K100="","",ROUND(K100*P100/100,2))</f>
+        <v/>
+      </c>
+      <c r="U100" s="4" t="str">
+        <f>IF(K100="","",ROUND(K100+M100+O100+Q100,2))</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   public/GST_Template.xlsx 	new file:   public/~$GST_Template.xlsx
</commit_message>
<xml_diff>
--- a/public/GST_Template.xlsx
+++ b/public/GST_Template.xlsx
@@ -160,7 +160,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
@@ -272,7 +273,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -297,6 +298,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,8 +690,8 @@
   </sheetPr>
   <dimension ref="A1:T100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:T6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,6 +783,31 @@
       <c r="A2" s="6"/>
       <c r="H2" s="7"/>
       <c r="K2" s="9"/>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>ROUND(K2*L2/100, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>ROUND(K2*N2/100, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>ROUND(K2*P2/100, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="10">
+        <f>K2+M2+O2+Q2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
@@ -807,19 +834,19 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="M7" t="str">
-        <f t="shared" ref="M2:M33" si="0">IF(K7="","",ROUND(K7*L7/100,2))</f>
+        <f t="shared" ref="M7:M33" si="0">IF(K7="","",ROUND(K7*L7/100,2))</f>
         <v/>
       </c>
       <c r="O7" t="str">
-        <f t="shared" ref="O2:O33" si="1">IF(K7="","",ROUND(K7*N7/100,2))</f>
+        <f t="shared" ref="O7:O33" si="1">IF(K7="","",ROUND(K7*N7/100,2))</f>
         <v/>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" ref="Q2:Q33" si="2">IF(K7="","",ROUND(K7*P7/100,2))</f>
+        <f t="shared" ref="Q7:Q33" si="2">IF(K7="","",ROUND(K7*P7/100,2))</f>
         <v/>
       </c>
       <c r="T7" t="str">
-        <f t="shared" ref="T2:T33" si="3">IF(K7="","",ROUND(K7+M7+O7+Q7,2))</f>
+        <f t="shared" ref="T7:T33" si="3">IF(K7="","",ROUND(K7+M7+O7+Q7,2))</f>
         <v/>
       </c>
     </row>

</xml_diff>